<commit_message>
Pequeñas modificaciones a tablas dinámicas
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegobeltran/Projects/Movies_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41F66B6-3FF4-9F4E-BF09-6D04FEF8E80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CB383A-1C17-594F-B03D-220F5CF1FF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13320" yWindow="500" windowWidth="27640" windowHeight="20840" activeTab="1" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
   </bookViews>
@@ -21,9 +21,8 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="904">
   <si>
     <t>ID</t>
   </si>
@@ -2793,6 +2792,9 @@
   </si>
   <si>
     <t>Hostal Ushuaia</t>
+  </si>
+  <si>
+    <t>View_place</t>
   </si>
 </sst>
 </file>
@@ -2801,7 +2803,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="173" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -2917,27 +2919,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="155">
+  <dxfs count="92">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <font>
+        <b val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2963,20 +2970,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2992,19 +2986,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="174" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -3020,10 +3002,10 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="174" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.0%"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -3036,17 +3018,10 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="173" formatCode="0.000"/>
     </dxf>
     <dxf>
       <font>
@@ -3059,12 +3034,10 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="173" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="172" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -3077,10 +3050,10 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="172" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.0%"/>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <font>
@@ -3093,20 +3066,10 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="0.0%"/>
+      <numFmt numFmtId="170" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <font>
@@ -3119,13 +3082,10 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="170" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.000%"/>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
     </dxf>
     <dxf>
       <font>
@@ -3138,13 +3098,10 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="0.000%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.0000%"/>
+      <numFmt numFmtId="169" formatCode="0.00000000"/>
     </dxf>
     <dxf>
       <font>
@@ -3157,13 +3114,10 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="169" formatCode="0.00000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.0000%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.000%"/>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
     </dxf>
     <dxf>
       <font>
@@ -3176,149 +3130,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.000%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
     </dxf>
     <dxf>
       <font>
@@ -3413,6 +3225,9 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
       </font>
@@ -3421,6 +3236,14 @@
       <font>
         <b val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -3444,109 +3267,10 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -3588,35 +3312,6 @@
       <font>
         <b val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -8488,8 +8183,341 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
-  <location ref="M3:N20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
+  <location ref="F3:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
+      <items count="16">
+        <item x="13"/>
+        <item x="2"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="%" fld="2" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="82">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="81">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="80">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="79">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
+  <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Avg_premiere_year" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="5">
+    <format dxfId="87">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="86">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="85">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="11" count="4">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="84">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="83">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
+  <location ref="M3:O14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField numFmtId="164" subtotalTop="0" showAll="0">
@@ -8537,7 +8565,7 @@
         </pivotArea>
       </autoSortScope>
     </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
       <items count="21">
         <item x="12"/>
         <item m="1" x="19"/>
@@ -8571,7 +8599,7 @@
         </pivotArea>
       </autoSortScope>
     </pivotField>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0">
       <items count="7">
         <item sd="0" x="0"/>
@@ -8598,7 +8626,7 @@
   <rowFields count="1">
     <field x="8"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="11">
     <i>
       <x v="5"/>
     </i>
@@ -8629,48 +8657,57 @@
     <i>
       <x v="8"/>
     </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x/>
-    </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
     <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <formats count="2">
-    <format dxfId="77">
+  <formats count="3">
+    <format dxfId="89">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
+  <filters count="2">
     <filter fld="5" type="count" evalOrder="-1" id="1" iMeasureFld="0">
       <autoFilter ref="A1">
         <filterColumn colId="0">
           <top10 val="10" filterVal="10"/>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+    <filter fld="8" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="greaterThan" val="1"/>
+          </customFilters>
         </filterColumn>
       </autoFilter>
     </filter>
@@ -8686,8 +8723,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
   <location ref="J3:K14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -9055,10 +9092,10 @@
     <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="97">
+    <format dxfId="91">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -9072,341 +9109,6 @@
       </autoFilter>
     </filter>
   </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
-  <location ref="F3:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
-      <items count="16">
-        <item x="13"/>
-        <item x="2"/>
-        <item x="14"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="12"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="%" fld="2" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="173"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="153">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="154">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="66">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="40">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
-  <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="11"/>
-    <field x="10"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Avg_premiere_year" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="5">
-    <format dxfId="111">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="112">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="113">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="11" count="4">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="114">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="115">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -9717,7 +9419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE35869-4E62-4D4B-8B4A-6A1A41B2E18E}">
   <dimension ref="A1:J345"/>
   <sheetViews>
-    <sheetView topLeftCell="A294" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I311" sqref="I311"/>
     </sheetView>
   </sheetViews>
@@ -20782,10 +20484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374D27D5-A834-CF47-BCCB-C52A324A5E45}">
-  <dimension ref="A2:N20"/>
+  <dimension ref="A2:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20802,9 +20504,10 @@
     <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.83203125" customWidth="1"/>
-    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.83203125" bestFit="1" customWidth="1"/>
@@ -20833,15 +20536,15 @@
     <col min="50" max="50" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>899</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>896</v>
       </c>
@@ -20870,416 +20573,414 @@
         <v>895</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>5</v>
+        <v>903</v>
       </c>
       <c r="N3" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="O3" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>891</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <v>84</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="16">
         <v>2006.7261904761904</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="16">
         <v>120.35714285714286</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4">
         <v>72</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="13">
         <v>0.20930232558139536</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4">
         <v>10</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="15">
         <v>291</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="O4" s="16">
+        <v>122.02405498281787</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>892</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>135</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="16">
         <v>1998.0222222222221</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="16">
         <v>118.49629629629629</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5">
         <v>71</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="13">
         <v>0.20639534883720931</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5">
         <v>6</v>
       </c>
       <c r="M5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="15">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="O5" s="16">
+        <v>123.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>893</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>90</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="16">
         <v>2005.3666666666666</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="16">
         <v>128.03333333333333</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6">
         <v>67</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="13">
         <v>0.19476744186046513</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6">
         <v>6</v>
       </c>
       <c r="M6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="16">
+      <c r="N6" s="15">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="O6" s="16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>894</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>35</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="16">
         <v>2012.0857142857142</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="16">
         <v>140.51428571428571</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7">
         <v>44</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="13">
         <v>0.12790697674418605</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7">
         <v>5</v>
       </c>
       <c r="M7" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="15">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="O7" s="16">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>890</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>344</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="16">
         <v>2003.5</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="16">
         <v>123.68604651162791</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8">
         <v>33</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="13">
         <v>9.5930232558139539E-2</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8">
         <v>5</v>
       </c>
       <c r="M8" s="12" t="s">
         <v>685</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="15">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="16">
+        <v>150.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F9" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9">
         <v>18</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="13">
         <v>5.232558139534884E-2</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9">
         <v>5</v>
       </c>
       <c r="M9" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="15">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="16">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F10" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10">
         <v>12</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="13">
         <v>3.4883720930232558E-2</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10">
         <v>5</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>578</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="15">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="16">
+        <v>142.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F11" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11">
         <v>11</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="13">
         <v>3.1976744186046513E-2</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>654</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11">
         <v>5</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>827</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="15">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="16">
+        <v>134.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F12" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12">
         <v>6</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="13">
         <v>1.7441860465116279E-2</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12">
         <v>4</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>625</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="15">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="16">
+        <v>142.33333333333334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F13" s="12" t="s">
         <v>604</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13">
         <v>3</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="13">
         <v>8.7209302325581394E-3</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13">
         <v>4</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="15">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="16">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F14" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14">
         <v>2</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="13">
         <v>5.8139534883720929E-3</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14">
         <v>55</v>
       </c>
-      <c r="M14" s="12" t="s">
-        <v>516</v>
-      </c>
-      <c r="N14" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" s="17" t="s">
+        <v>890</v>
+      </c>
+      <c r="N14" s="15">
+        <v>338</v>
+      </c>
+      <c r="O14" s="16">
+        <v>123.22485207100591</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F15" s="12" t="s">
         <v>577</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15">
         <v>2</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="13">
         <v>5.8139534883720929E-3</v>
       </c>
-      <c r="M15" s="12" t="s">
-        <v>661</v>
-      </c>
-      <c r="N15" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F16" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="13">
         <v>2.9069767441860465E-3</v>
       </c>
-      <c r="M16" s="12" t="s">
-        <v>570</v>
-      </c>
-      <c r="N16" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="6:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F17" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="13">
         <v>2.9069767441860465E-3</v>
       </c>
-      <c r="M17" s="12" t="s">
-        <v>902</v>
-      </c>
-      <c r="N17" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="6:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F18" s="12" t="s">
         <v>660</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="13">
         <v>2.9069767441860465E-3</v>
       </c>
-      <c r="M18" s="12" t="s">
-        <v>877</v>
-      </c>
-      <c r="N18" s="16">
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F19" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="G19">
+        <v>344</v>
+      </c>
+      <c r="H19" s="13">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="F19" s="15" t="s">
-        <v>890</v>
-      </c>
-      <c r="G19" s="16">
-        <v>344</v>
-      </c>
-      <c r="H19" s="17">
-        <v>1</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>717</v>
-      </c>
-      <c r="N19" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="M20" s="15" t="s">
-        <v>890</v>
-      </c>
-      <c r="N20" s="16">
-        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadiendo el análisis por plataforma
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -8,21 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegobeltran/Projects/Movies_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646EC9C8-FA40-5D46-9EF0-779C08E2E452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BF6D37-33B9-BB4A-84F2-9FCD4EF9DD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13320" yWindow="500" windowWidth="27640" windowHeight="20840" activeTab="1" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
+    <workbookView xWindow="13320" yWindow="500" windowWidth="27640" windowHeight="20840" activeTab="2" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="1" r:id="rId1"/>
-    <sheet name="View_Analysis" sheetId="3" r:id="rId2"/>
-    <sheet name="Pivot_Tables" sheetId="2" r:id="rId3"/>
+    <sheet name="Pivot_Tables" sheetId="2" r:id="rId2"/>
+    <sheet name="View_Analysis" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Movies!$A$1:$M$345</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">View_Analysis!$A$38:$A$52</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">View_Analysis!$B$37</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">View_Analysis!$B$37</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">View_Analysis!$A$38:$A$52</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">View_Analysis!$B$37</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">View_Analysis!$A$38:$A$52</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">View_Analysis!$B$37</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">View_Analysis!$A$38:$A$52</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">View_Analysis!$B$37</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">View_Analysis!$A$38:$A$52</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">View_Analysis!$B$37</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">View_Analysis!$A$38:$A$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="937">
   <si>
     <t>ID</t>
   </si>
@@ -2819,9 +2837,6 @@
     <t>View count / month</t>
   </si>
   <si>
-    <t>Week day</t>
-  </si>
-  <si>
     <t>Nº Month</t>
   </si>
   <si>
@@ -2861,12 +2876,6 @@
     <t>December</t>
   </si>
   <si>
-    <t>Nº Week day</t>
-  </si>
-  <si>
-    <t>View count / week day</t>
-  </si>
-  <si>
     <t>Sunday</t>
   </si>
   <si>
@@ -2886,6 +2895,24 @@
   </si>
   <si>
     <t>Saturday</t>
+  </si>
+  <si>
+    <t>Day of week</t>
+  </si>
+  <si>
+    <t>Nº Day of week</t>
+  </si>
+  <si>
+    <t>View count / day of week</t>
+  </si>
+  <si>
+    <t>DATE STATISTICS</t>
+  </si>
+  <si>
+    <t>View count / platform</t>
+  </si>
+  <si>
+    <t>PLATFORM / YEAR</t>
   </si>
 </sst>
 </file>
@@ -2896,7 +2923,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2944,8 +2971,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2960,7 +2995,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2992,7 +3033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3030,24 +3071,152 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF70AD47"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3113,39 +3282,12 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -3156,14 +3298,12 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -3215,8 +3355,23 @@
         <b val="0"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF70AD47"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3235,10 +3390,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="108"/>
+      <c14:style val="106"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="8"/>
+      <c:style val="6"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -3251,7 +3406,7 @@
             <a:pPr>
               <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3259,7 +3414,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-MX"/>
+              <a:rPr lang="es-MX">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Movies watched per year</a:t>
             </a:r>
           </a:p>
@@ -3280,7 +3439,7 @@
           <a:pPr>
             <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3305,11 +3464,12 @@
               <a:solidFill>
                 <a:schemeClr val="lt1"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
-                <a:schemeClr val="accent6">
+                <a:schemeClr val="accent4">
                   <a:tint val="65000"/>
                 </a:schemeClr>
               </a:outerShdw>
@@ -3335,7 +3495,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3360,7 +3520,7 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent6">
+                        <a:schemeClr val="accent4">
                           <a:lumMod val="60000"/>
                           <a:lumOff val="40000"/>
                         </a:schemeClr>
@@ -3374,7 +3534,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>View_Analysis!$A$2:$A$5</c:f>
+              <c:f>View_Analysis!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3395,7 +3555,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>View_Analysis!$B$2:$B$5</c:f>
+              <c:f>View_Analysis!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3446,6 +3606,7 @@
                 </a:gsLst>
                 <a:lin ang="5400000" scaled="0"/>
               </a:gradFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3483,7 +3644,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3560,11 +3721,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="accent6"/>
+      <a:schemeClr val="accent4"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="accent6"/>
+        <a:schemeClr val="accent4"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -3595,10 +3756,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="104"/>
+      <c14:style val="106"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="4"/>
+      <c:style val="6"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -3618,7 +3779,7 @@
           <a:pPr>
             <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3641,7 +3802,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>View_Analysis!$E$1</c:f>
+              <c:f>View_Analysis!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3653,7 +3814,7 @@
           <c:spPr>
             <a:pattFill prst="ltUpDiag">
               <a:fgClr>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:fgClr>
               <a:bgClr>
                 <a:schemeClr val="lt1"/>
@@ -3668,7 +3829,7 @@
           <c:dLbls>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent4">
                   <a:alpha val="70000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -3684,9 +3845,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3711,7 +3872,7 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent2">
+                        <a:schemeClr val="accent4">
                           <a:lumMod val="60000"/>
                           <a:lumOff val="40000"/>
                         </a:schemeClr>
@@ -3725,7 +3886,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>View_Analysis!$D$2:$D$13</c:f>
+              <c:f>View_Analysis!$D$3:$D$14</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -3769,7 +3930,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>View_Analysis!$E$2:$E$13</c:f>
+              <c:f>View_Analysis!$E$3:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3847,7 +4008,7 @@
           <a:noFill/>
           <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="accent2">
+              <a:schemeClr val="accent4">
                 <a:lumMod val="60000"/>
                 <a:lumOff val="40000"/>
               </a:schemeClr>
@@ -3863,7 +4024,7 @@
             <a:pPr>
               <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3953,11 +4114,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="accent2"/>
+      <a:schemeClr val="accent4"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="accent2"/>
+        <a:schemeClr val="accent4"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -4034,11 +4195,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>View_Analysis!$H$1</c:f>
+              <c:f>View_Analysis!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>View count / week day</c:v>
+                  <c:v>View count / day of week</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4118,7 +4279,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>View_Analysis!$G$2:$G$8</c:f>
+              <c:f>View_Analysis!$G$3:$G$9</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -4147,7 +4308,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>View_Analysis!$H$2:$H$8</c:f>
+              <c:f>View_Analysis!$H$3:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4344,21 +4505,149 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v2.6</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>PLATFORMS USE</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1600" b="1" i="0" u="none" strike="noStrike" spc="100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="95000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>PLATFORMS USE</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="funnel" uniqueId="{2C5229B8-BD96-2F40-9319-DB298067D9B7}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v2.7</cx:f>
+              <cx:v>View count / platform</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels>
+            <cx:txPr>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+            <cx:separator>, </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="1">
+        <cx:catScaling gapWidth="0.0599999987"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
-  <a:schemeClr val="accent6"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
-  <a:schemeClr val="accent2"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -5963,20 +6252,561 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="427">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" spc="100">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6004,15 +6834,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6039,16 +6869,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6071,6 +6901,84 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>82549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>14110</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Gráfico 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3434528-6C54-B389-2D94-D1C18C1D5165}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6338006" y="7236882"/>
+              <a:ext cx="6305550" cy="4320117"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-MX" sz="1100"/>
+                <a:t>Este gráfico no está disponible en tu versión de Excel.
+Si editas esta forma o guardas el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10923,7 +11831,548 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
+  <location ref="F3:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
+      <items count="16">
+        <item x="13"/>
+        <item x="2"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="%" fld="2" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="21">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
+  <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Avg_premiere_year" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="5">
+    <format dxfId="26">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="11" count="4">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
+  <location ref="M3:O14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0" sortType="descending">
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
+      <items count="21">
+        <item x="12"/>
+        <item m="1" x="19"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item m="1" x="17"/>
+        <item x="0"/>
+        <item m="1" x="18"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item m="1" x="16"/>
+        <item x="14"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="29">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="28">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="27">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="2">
+    <filter fld="5" type="count" evalOrder="-1" id="1" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <top10 val="10" filterVal="10"/>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+    <filter fld="8" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="greaterThan" val="1"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
   <location ref="J3:K14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -11291,10 +12740,10 @@
     <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="11">
+    <format dxfId="31">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -11319,562 +12768,48 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
-  <location ref="F3:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
-      <items count="16">
-        <item x="13"/>
-        <item x="2"/>
-        <item x="14"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="12"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="%" fld="2" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="165"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="15">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="14">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A4A6DBB-95E5-F349-B30E-01F5E818A101}" name="Tabla1" displayName="Tabla1" ref="A2:H14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="17">
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{A5A5E420-8F02-0C4A-8221-CB3D62B2C5D9}" name="Year" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E3ADC4E5-1669-7243-A25F-9784ABBCA501}" name="View count / year" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{C6222808-140C-5743-B272-A6EA41F2B28D}" name="Nº Month" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{AEB3E933-8585-B140-9D83-AD2ED76F835D}" name="Month" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{E881D891-37C9-A54A-A0F7-2F1937B43161}" name="View count / month" dataDxfId="12">
+      <calculatedColumnFormula>COUNTIF(Movies!D:D,View_Analysis!C3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{9291B7F2-C047-A245-A570-3E65956C06C0}" name="Nº Day of week" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{E63B61D0-FB2A-6543-ABF7-A5A1337847A3}" name="Day of week" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{183AD3B2-31A7-724A-BD7A-6223328AFB58}" name="View count / day of week" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
-  <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Avg_premiere_year" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="5">
-    <format dxfId="20">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="11" count="4">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="17">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="16">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
-  <location ref="M3:O14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0" sortType="descending">
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
-      <items count="21">
-        <item x="12"/>
-        <item m="1" x="19"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item m="1" x="17"/>
-        <item x="0"/>
-        <item m="1" x="18"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="11"/>
-        <item m="1" x="16"/>
-        <item x="14"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="15"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="23">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="22">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="21">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="2">
-    <filter fld="5" type="count" evalOrder="-1" id="1" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <top10 val="10" filterVal="10"/>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-    <filter fld="8" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThan" val="1"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A4A6DBB-95E5-F349-B30E-01F5E818A101}" name="Tabla1" displayName="Tabla1" ref="A1:H13" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A5A5E420-8F02-0C4A-8221-CB3D62B2C5D9}" name="Year" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{E3ADC4E5-1669-7243-A25F-9784ABBCA501}" name="View count / year" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C6222808-140C-5743-B272-A6EA41F2B28D}" name="Nº Month" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{AEB3E933-8585-B140-9D83-AD2ED76F835D}" name="Month" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E881D891-37C9-A54A-A0F7-2F1937B43161}" name="View count / month" dataDxfId="3">
-      <calculatedColumnFormula>COUNTIF(Movies!D:D,View_Analysis!C2)</calculatedColumnFormula>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B41941F1-754D-FE4C-8D12-1FA64515E1EF}" name="Tabla13" displayName="Tabla13" ref="A37:F52" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:F52">
+    <sortCondition descending="1" ref="B38:B52"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{33520D8E-AE00-9D41-8882-149DBBA1153C}" name="Platform" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{6A682448-B962-BE40-A0D0-BA72854AF347}" name="View count / platform" dataDxfId="7">
+      <calculatedColumnFormula>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9291B7F2-C047-A245-A570-3E65956C06C0}" name="Nº Week day" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{E63B61D0-FB2A-6543-ABF7-A5A1337847A3}" name="Week day" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{183AD3B2-31A7-724A-BD7A-6223328AFB58}" name="View count / week day" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{132BBAB9-8C4C-D14F-9A5A-A9ABAA5AE951}" name="2020" dataDxfId="4">
+      <calculatedColumnFormula>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{5ED70BDD-3B26-ED46-8C04-B73F9AC9A830}" name="2021" dataDxfId="3">
+      <calculatedColumnFormula>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{64A7D1C9-47E2-6448-BBC9-A5F0D98380C0}" name="2022" dataDxfId="2">
+      <calculatedColumnFormula>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E779A56B-D75B-0941-9B7C-5C6B1154326F}" name="2023" dataDxfId="1">
+      <calculatedColumnFormula>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -12177,8 +13112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE35869-4E62-4D4B-8B4A-6A1A41B2E18E}">
   <dimension ref="A1:M345"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="C1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27381,339 +28316,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE8EAA1-17E3-2941-BDE2-1625C2DA10AF}">
-  <dimension ref="A1:H13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>907</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>908</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>912</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>909</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>910</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>925</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>911</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="17">
-        <v>2020</v>
-      </c>
-      <c r="B2" s="17">
-        <f>COUNTIF(Movies!C:C,View_Analysis!A2)</f>
-        <v>84</v>
-      </c>
-      <c r="C2" s="17">
-        <v>1</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>913</v>
-      </c>
-      <c r="E2" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C2)</f>
-        <v>45</v>
-      </c>
-      <c r="F2" s="17">
-        <v>1</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>927</v>
-      </c>
-      <c r="H2" s="17">
-        <f>COUNTIF(Movies!E:E,View_Analysis!F2)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
-        <v>2021</v>
-      </c>
-      <c r="B3" s="17">
-        <f>COUNTIF(Movies!C:C,View_Analysis!A3)</f>
-        <v>135</v>
-      </c>
-      <c r="C3" s="17">
-        <v>2</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>914</v>
-      </c>
-      <c r="E3" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C3)</f>
-        <v>31</v>
-      </c>
-      <c r="F3" s="17">
-        <v>2</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>928</v>
-      </c>
-      <c r="H3" s="17">
-        <f>COUNTIF(Movies!E:E,View_Analysis!F3)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="17">
-        <v>2022</v>
-      </c>
-      <c r="B4" s="17">
-        <f>COUNTIF(Movies!C:C,View_Analysis!A4)</f>
-        <v>90</v>
-      </c>
-      <c r="C4" s="17">
-        <v>3</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>915</v>
-      </c>
-      <c r="E4" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C4)</f>
-        <v>32</v>
-      </c>
-      <c r="F4" s="17">
-        <v>3</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>929</v>
-      </c>
-      <c r="H4" s="17">
-        <f>COUNTIF(Movies!E:E,View_Analysis!F4)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
-        <v>2023</v>
-      </c>
-      <c r="B5" s="17">
-        <f>COUNTIF(Movies!C:C,View_Analysis!A5)</f>
-        <v>35</v>
-      </c>
-      <c r="C5" s="17">
-        <v>4</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>916</v>
-      </c>
-      <c r="E5" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C5)</f>
-        <v>54</v>
-      </c>
-      <c r="F5" s="17">
-        <v>4</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>930</v>
-      </c>
-      <c r="H5" s="17">
-        <f>COUNTIF(Movies!E:E,View_Analysis!F5)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17">
-        <v>5</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>917</v>
-      </c>
-      <c r="E6" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C6)</f>
-        <v>38</v>
-      </c>
-      <c r="F6" s="17">
-        <v>5</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="H6" s="17">
-        <f>COUNTIF(Movies!E:E,View_Analysis!F6)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17">
-        <v>6</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>918</v>
-      </c>
-      <c r="E7" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C7)</f>
-        <v>27</v>
-      </c>
-      <c r="F7" s="17">
-        <v>6</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>932</v>
-      </c>
-      <c r="H7" s="17">
-        <f>COUNTIF(Movies!E:E,View_Analysis!F7)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17">
-        <v>7</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>919</v>
-      </c>
-      <c r="E8" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C8)</f>
-        <v>26</v>
-      </c>
-      <c r="F8" s="17">
-        <v>7</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>933</v>
-      </c>
-      <c r="H8" s="17">
-        <f>COUNTIF(Movies!E:E,View_Analysis!F8)</f>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17">
-        <v>8</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>920</v>
-      </c>
-      <c r="E9" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C9)</f>
-        <v>22</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17">
-        <v>9</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>921</v>
-      </c>
-      <c r="E10" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C10)</f>
-        <v>17</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17">
-        <v>10</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>922</v>
-      </c>
-      <c r="E11" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C11)</f>
-        <v>18</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17">
-        <v>11</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>923</v>
-      </c>
-      <c r="E12" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C12)</f>
-        <v>14</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17">
-        <v>12</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>924</v>
-      </c>
-      <c r="E13" s="17">
-        <f>COUNTIF(Movies!D:D,View_Analysis!C13)</f>
-        <v>20</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374D27D5-A834-CF47-BCCB-C52A324A5E45}">
   <dimension ref="A2:O19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F4" sqref="F4:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27763,12 +28370,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>899</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -28215,4 +28822,762 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE8EAA1-17E3-2941-BDE2-1625C2DA10AF}">
+  <dimension ref="A1:K52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>934</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>907</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>908</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>911</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>909</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>910</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>932</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>931</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="16">
+        <f>COUNTIF(Movies!C:C,View_Analysis!A3)</f>
+        <v>84</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>912</v>
+      </c>
+      <c r="E3" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C3)</f>
+        <v>45</v>
+      </c>
+      <c r="F3" s="16">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>924</v>
+      </c>
+      <c r="H3" s="16">
+        <f>COUNTIF(Movies!E:E,View_Analysis!F3)</f>
+        <v>48</v>
+      </c>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="16">
+        <f>COUNTIF(Movies!C:C,View_Analysis!A4)</f>
+        <v>135</v>
+      </c>
+      <c r="C4" s="16">
+        <v>2</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="E4" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C4)</f>
+        <v>31</v>
+      </c>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>925</v>
+      </c>
+      <c r="H4" s="16">
+        <f>COUNTIF(Movies!E:E,View_Analysis!F4)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="16">
+        <v>2022</v>
+      </c>
+      <c r="B5" s="16">
+        <f>COUNTIF(Movies!C:C,View_Analysis!A5)</f>
+        <v>90</v>
+      </c>
+      <c r="C5" s="16">
+        <v>3</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>914</v>
+      </c>
+      <c r="E5" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C5)</f>
+        <v>32</v>
+      </c>
+      <c r="F5" s="16">
+        <v>3</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>926</v>
+      </c>
+      <c r="H5" s="16">
+        <f>COUNTIF(Movies!E:E,View_Analysis!F5)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>2023</v>
+      </c>
+      <c r="B6" s="16">
+        <f>COUNTIF(Movies!C:C,View_Analysis!A6)</f>
+        <v>35</v>
+      </c>
+      <c r="C6" s="16">
+        <v>4</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>915</v>
+      </c>
+      <c r="E6" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C6)</f>
+        <v>54</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>927</v>
+      </c>
+      <c r="H6" s="16">
+        <f>COUNTIF(Movies!E:E,View_Analysis!F6)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16">
+        <v>5</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>916</v>
+      </c>
+      <c r="E7" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C7)</f>
+        <v>38</v>
+      </c>
+      <c r="F7" s="16">
+        <v>5</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="H7" s="16">
+        <f>COUNTIF(Movies!E:E,View_Analysis!F7)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>917</v>
+      </c>
+      <c r="E8" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C8)</f>
+        <v>27</v>
+      </c>
+      <c r="F8" s="16">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>929</v>
+      </c>
+      <c r="H8" s="16">
+        <f>COUNTIF(Movies!E:E,View_Analysis!F8)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16">
+        <v>7</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>918</v>
+      </c>
+      <c r="E9" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C9)</f>
+        <v>26</v>
+      </c>
+      <c r="F9" s="16">
+        <v>7</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>930</v>
+      </c>
+      <c r="H9" s="16">
+        <f>COUNTIF(Movies!E:E,View_Analysis!F9)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16">
+        <v>8</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="E10" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C10)</f>
+        <v>22</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16">
+        <v>9</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>920</v>
+      </c>
+      <c r="E11" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C11)</f>
+        <v>17</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16">
+        <v>10</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>921</v>
+      </c>
+      <c r="E12" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C12)</f>
+        <v>18</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16">
+        <v>11</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>922</v>
+      </c>
+      <c r="E13" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C13)</f>
+        <v>14</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16">
+        <v>12</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>923</v>
+      </c>
+      <c r="E14" s="16">
+        <f>COUNTIF(Movies!D:D,View_Analysis!C14)</f>
+        <v>20</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>936</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="23" t="s">
+        <v>900</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>935</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>891</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>892</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>893</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>72</v>
+      </c>
+      <c r="C38" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>30</v>
+      </c>
+      <c r="D38" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>23</v>
+      </c>
+      <c r="E38" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>16</v>
+      </c>
+      <c r="F38" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>71</v>
+      </c>
+      <c r="C39" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>28</v>
+      </c>
+      <c r="D39" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>24</v>
+      </c>
+      <c r="E39" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>15</v>
+      </c>
+      <c r="F39" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>67</v>
+      </c>
+      <c r="C40" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>16</v>
+      </c>
+      <c r="D40" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>26</v>
+      </c>
+      <c r="E40" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>18</v>
+      </c>
+      <c r="F40" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B41" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>44</v>
+      </c>
+      <c r="C41" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>4</v>
+      </c>
+      <c r="D41" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>23</v>
+      </c>
+      <c r="E41" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>16</v>
+      </c>
+      <c r="F41" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>33</v>
+      </c>
+      <c r="C42" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>4</v>
+      </c>
+      <c r="D42" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>10</v>
+      </c>
+      <c r="E42" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>12</v>
+      </c>
+      <c r="F42" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="B43" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>18</v>
+      </c>
+      <c r="C43" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>15</v>
+      </c>
+      <c r="E43" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>3</v>
+      </c>
+      <c r="F43" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B44" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>12</v>
+      </c>
+      <c r="C44" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>2</v>
+      </c>
+      <c r="D44" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>5</v>
+      </c>
+      <c r="E44" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>2</v>
+      </c>
+      <c r="F44" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="B45" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>11</v>
+      </c>
+      <c r="C45" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>4</v>
+      </c>
+      <c r="E45" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>3</v>
+      </c>
+      <c r="F45" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="B46" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>6</v>
+      </c>
+      <c r="C46" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>2</v>
+      </c>
+      <c r="F46" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="B47" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>3</v>
+      </c>
+      <c r="C47" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>2</v>
+      </c>
+      <c r="F47" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>577</v>
+      </c>
+      <c r="B48" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>2</v>
+      </c>
+      <c r="C48" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>2</v>
+      </c>
+      <c r="E48" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="B49" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>2</v>
+      </c>
+      <c r="C49" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>1</v>
+      </c>
+      <c r="E49" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
+        <v>660</v>
+      </c>
+      <c r="B50" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>1</v>
+      </c>
+      <c r="C50" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D50" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>1</v>
+      </c>
+      <c r="F50" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B51" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>1</v>
+      </c>
+      <c r="C51" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>1</v>
+      </c>
+      <c r="E51" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B52" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</f>
+        <v>1</v>
+      </c>
+      <c r="C52" s="16">
+        <f>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</f>
+        <v>1</v>
+      </c>
+      <c r="E52" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="16">
+        <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A36:F36"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B38" calculatedColumn="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Incorporación de la índice y coincidir para comparar dos plataformas por año
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegobeltran/Projects/Movies_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BF6D37-33B9-BB4A-84F2-9FCD4EF9DD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD1ABD3-F5BE-FE4B-A2F7-8B97327F68AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13320" yWindow="500" windowWidth="27640" windowHeight="20840" activeTab="2" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
   </bookViews>
@@ -19,28 +19,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Movies!$A$1:$M$345</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">View_Analysis!$A$38:$A$52</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">View_Analysis!$B$37</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">View_Analysis!$B$37</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">View_Analysis!$B$38:$B$52</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">View_Analysis!$A$38:$A$52</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">View_Analysis!$B$37</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">View_Analysis!$B$38:$B$52</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">View_Analysis!$A$38:$A$52</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">View_Analysis!$B$37</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">View_Analysis!$B$38:$B$52</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">View_Analysis!$A$60</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">View_Analysis!$B$58:$C$59</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">View_Analysis!$B$60:$C$60</definedName>
     <definedName name="_xlchart.v2.3" hidden="1">View_Analysis!$A$38:$A$52</definedName>
     <definedName name="_xlchart.v2.4" hidden="1">View_Analysis!$B$37</definedName>
     <definedName name="_xlchart.v2.5" hidden="1">View_Analysis!$B$38:$B$52</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">View_Analysis!$A$38:$A$52</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">View_Analysis!$B$37</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">View_Analysis!$B$38:$B$52</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">View_Analysis!$A$38:$A$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -62,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="938">
   <si>
     <t>ID</t>
   </si>
@@ -2913,6 +2901,9 @@
   </si>
   <si>
     <t>PLATFORM / YEAR</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -3075,14 +3066,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3090,53 +3075,24 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF70AD47"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3180,7 +3136,23 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3202,7 +3174,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF70AD47"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3290,20 +3262,49 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -3344,16 +3345,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -4505,15 +4496,397 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="95000"/>
+                    <a:lumOff val="5000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="95000"/>
+                    <a:lumOff val="5000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>platform comparative / year</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>View_Analysis!$A$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent3"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="lt1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="95000"/>
+                        <a:lumOff val="5000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CO"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3">
+                          <a:lumMod val="60000"/>
+                          <a:lumOff val="40000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>View_Analysis!$B$58:$C$59</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Cine Colombia</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Netflix</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2022</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>View_Analysis!$B$60:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8369-A044-8861-3499AF9C3592}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:overlap val="-20"/>
+        <c:axId val="2112505567"/>
+        <c:axId val="2112507567"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2112505567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="95000"/>
+                    <a:lumOff val="5000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2112507567"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2112507567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="95000"/>
+                    <a:lumOff val="5000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2112505567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent3"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent3"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v2.6</cx:f>
+        <cx:f>_xlchart.v2.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v2.8</cx:f>
+        <cx:f>_xlchart.v2.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4557,7 +4930,7 @@
         <cx:series layoutId="funnel" uniqueId="{2C5229B8-BD96-2F40-9319-DB298067D9B7}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v2.7</cx:f>
+              <cx:f>_xlchart.v2.4</cx:f>
               <cx:v>View count / platform</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4587,7 +4960,7 @@
           <cx:dataId val="0"/>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="1">
+      <cx:axis id="0">
         <cx:catScaling gapWidth="0.0599999987"/>
         <cx:tickLabels/>
       </cx:axis>
@@ -4648,6 +5021,12 @@
     <a:lumMod val="50000"/>
     <a:lumOff val="50000"/>
   </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
+  <a:schemeClr val="accent3"/>
 </cs:colorStyle>
 </file>
 
@@ -6793,6 +7172,542 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="226">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6950,8 +7865,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6338006" y="7236882"/>
-              <a:ext cx="6305550" cy="4320117"/>
+              <a:off x="6343650" y="7423149"/>
+              <a:ext cx="6280150" cy="4427361"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6979,6 +7894,42 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>18345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>712612</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>193323</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A71A60-DAFA-8199-55D9-CED58F17B8A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -11831,548 +12782,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
-  <location ref="F3:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
-      <items count="16">
-        <item x="13"/>
-        <item x="2"/>
-        <item x="14"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="12"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="%" fld="2" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="165"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="21">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="20">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="19">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="18">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
-  <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Avg_premiere_year" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="5">
-    <format dxfId="26">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="24">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="11" count="4">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="22">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
-  <location ref="M3:O14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0" sortType="descending">
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
-      <items count="21">
-        <item x="12"/>
-        <item m="1" x="19"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item m="1" x="17"/>
-        <item x="0"/>
-        <item m="1" x="18"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="11"/>
-        <item m="1" x="16"/>
-        <item x="14"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="15"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="29">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="28">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="27">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="2">
-    <filter fld="5" type="count" evalOrder="-1" id="1" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <top10 val="10" filterVal="10"/>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-    <filter fld="8" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThan" val="1"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
   <location ref="J3:K14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -12740,10 +13150,10 @@
     <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="31">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -12768,44 +13178,585 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
+  <location ref="F3:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
+      <items count="16">
+        <item x="13"/>
+        <item x="2"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="%" fld="2" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="23">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="21">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
+  <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Avg_premiere_year" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="5">
+    <format dxfId="28">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="11" count="4">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
+  <location ref="M3:O14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0" sortType="descending">
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" measureFilter="1" sortType="descending">
+      <items count="21">
+        <item x="12"/>
+        <item m="1" x="19"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item m="1" x="17"/>
+        <item x="0"/>
+        <item m="1" x="18"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item m="1" x="16"/>
+        <item x="14"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count_view" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Avg_duration(min)" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="31">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="29">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium10" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="2">
+    <filter fld="5" type="count" evalOrder="-1" id="1" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <top10 val="10" filterVal="10"/>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+    <filter fld="8" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="greaterThan" val="1"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A4A6DBB-95E5-F349-B30E-01F5E818A101}" name="Tabla1" displayName="Tabla1" ref="A2:H14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A4A6DBB-95E5-F349-B30E-01F5E818A101}" name="Tabla1" displayName="Tabla1" ref="A2:H14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A5A5E420-8F02-0C4A-8221-CB3D62B2C5D9}" name="Year" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{E3ADC4E5-1669-7243-A25F-9784ABBCA501}" name="View count / year" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{C6222808-140C-5743-B272-A6EA41F2B28D}" name="Nº Month" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{AEB3E933-8585-B140-9D83-AD2ED76F835D}" name="Month" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{E881D891-37C9-A54A-A0F7-2F1937B43161}" name="View count / month" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{A5A5E420-8F02-0C4A-8221-CB3D62B2C5D9}" name="Year" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E3ADC4E5-1669-7243-A25F-9784ABBCA501}" name="View count / year" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{C6222808-140C-5743-B272-A6EA41F2B28D}" name="Nº Month" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{AEB3E933-8585-B140-9D83-AD2ED76F835D}" name="Month" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{E881D891-37C9-A54A-A0F7-2F1937B43161}" name="View count / month" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(Movies!D:D,View_Analysis!C3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9291B7F2-C047-A245-A570-3E65956C06C0}" name="Nº Day of week" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{E63B61D0-FB2A-6543-ABF7-A5A1337847A3}" name="Day of week" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{183AD3B2-31A7-724A-BD7A-6223328AFB58}" name="View count / day of week" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{9291B7F2-C047-A245-A570-3E65956C06C0}" name="Nº Day of week" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{E63B61D0-FB2A-6543-ABF7-A5A1337847A3}" name="Day of week" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{183AD3B2-31A7-724A-BD7A-6223328AFB58}" name="View count / day of week" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B41941F1-754D-FE4C-8D12-1FA64515E1EF}" name="Tabla13" displayName="Tabla13" ref="A37:F52" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B41941F1-754D-FE4C-8D12-1FA64515E1EF}" name="Tabla13" displayName="Tabla13" ref="A37:F52" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:F52">
     <sortCondition descending="1" ref="B38:B52"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{33520D8E-AE00-9D41-8882-149DBBA1153C}" name="Platform" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{6A682448-B962-BE40-A0D0-BA72854AF347}" name="View count / platform" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{6A682448-B962-BE40-A0D0-BA72854AF347}" name="View count / platform" dataDxfId="4">
       <calculatedColumnFormula>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{132BBAB9-8C4C-D14F-9A5A-A9ABAA5AE951}" name="2020" dataDxfId="4">
+    <tableColumn id="10" xr3:uid="{132BBAB9-8C4C-D14F-9A5A-A9ABAA5AE951}" name="2020" dataDxfId="3">
       <calculatedColumnFormula>COUNTIFS(Movies!$K:$K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2020]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{5ED70BDD-3B26-ED46-8C04-B73F9AC9A830}" name="2021" dataDxfId="3">
+    <tableColumn id="11" xr3:uid="{5ED70BDD-3B26-ED46-8C04-B73F9AC9A830}" name="2021" dataDxfId="2">
       <calculatedColumnFormula>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2021]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{64A7D1C9-47E2-6448-BBC9-A5F0D98380C0}" name="2022" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{64A7D1C9-47E2-6448-BBC9-A5F0D98380C0}" name="2022" dataDxfId="1">
       <calculatedColumnFormula>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2022]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E779A56B-D75B-0941-9B7C-5C6B1154326F}" name="2023" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{E779A56B-D75B-0941-9B7C-5C6B1154326F}" name="2023" dataDxfId="0">
       <calculatedColumnFormula>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -28370,12 +29321,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="23" t="s">
         <v>899</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -28826,10 +29777,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE8EAA1-17E3-2941-BDE2-1625C2DA10AF}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28846,40 +29797,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>934</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:11" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>907</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>908</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>911</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>909</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>910</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>932</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="18" t="s">
         <v>931</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="19" t="s">
         <v>933</v>
       </c>
     </row>
@@ -28911,7 +29862,7 @@
         <f>COUNTIF(Movies!E:E,View_Analysis!F3)</f>
         <v>48</v>
       </c>
-      <c r="K3" s="18"/>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
@@ -29158,34 +30109,34 @@
       <c r="H14" s="16"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="24" t="s">
         <v>936</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="21" t="s">
         <v>900</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="22" t="s">
         <v>935</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="22" t="s">
         <v>891</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="22" t="s">
         <v>892</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="21" t="s">
         <v>893</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="21" t="s">
         <v>894</v>
       </c>
     </row>
@@ -29562,6 +30513,38 @@
       <c r="F52" s="16">
         <f>COUNTIFS(Movies!K:K,Tabla13[[#This Row],[Platform]],Movies!C:C,Tabla13[[#Headers],[2023]])</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>907</v>
+      </c>
+      <c r="B58" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>900</v>
+      </c>
+      <c r="B59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>937</v>
+      </c>
+      <c r="B60">
+        <f>INDEX(Tabla13[[2020]:[2023]],MATCH(B59,Tabla13[Platform],0),MATCH(B58,Tabla13[[#Headers],[2020]:[2023]],0))</f>
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <f>INDEX(Tabla13[[2020]:[2023]],MATCH(C59,Tabla13[Platform],0),MATCH(B58,Tabla13[[#Headers],[2020]:[2023]],0))</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -29570,6 +30553,14 @@
     <mergeCell ref="A36:F36"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59 C59" xr:uid="{5C8CC8B5-37F4-1C49-922D-16EF357A1744}">
+      <formula1>$A$38:$A$52</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58" xr:uid="{BF5E9006-DA2A-884A-8647-AE2DC2EC2F15}">
+      <formula1>$C$37:$F$37</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="B38" calculatedColumn="1"/>

</xml_diff>

<commit_message>
Borrador del dashboard por plataforma
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -8,25 +8,54 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegobeltran/Projects/Movies_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C31B4F-4908-5344-A31B-8D802C6050E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C1788F-C29C-244A-99F1-F6D468DB92B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12580" yWindow="500" windowWidth="28160" windowHeight="20840" activeTab="3" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
+    <workbookView xWindow="12580" yWindow="500" windowWidth="28160" windowHeight="20840" activeTab="4" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot_Tables" sheetId="2" r:id="rId2"/>
     <sheet name="View_Analysis" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="Dashboard-1" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Hoja1!$A$1:$Y$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Movies!$A$1:$O$345</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$B$41</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$B$42:$B$43</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$A$42:$A$43</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$B$41</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$B$42:$B$43</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Hoja1!$A$4:$A$18</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Hoja1!$B$3</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Hoja1!$B$4:$B$18</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Hoja1!$A$4:$A$18</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Hoja1!$B$3</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Hoja1!$B$4:$B$18</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Hoja1!$A$42:$A$43</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Hoja1!$B$41</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Hoja1!$B$42:$B$43</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Hoja1!$A$42:$A$43</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Hoja1!$B$41</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Hoja1!$B$42:$B$43</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$A$42:$A$43</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$B$41</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$B$42:$B$43</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$A$42:$A$43</definedName>
     <definedName name="_xlchart.v2.0" hidden="1">View_Analysis!$A$38:$A$52</definedName>
     <definedName name="_xlchart.v2.1" hidden="1">View_Analysis!$B$37</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">Hoja1!$A$4:$A$18</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">Hoja1!$B$3</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">Hoja1!$B$4:$B$18</definedName>
     <definedName name="_xlchart.v2.2" hidden="1">View_Analysis!$B$38:$B$52</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Hoja1!$A$4:$A$18</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Hoja1!$B$3</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">Hoja1!$B$4:$B$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="974">
   <si>
     <t>ID</t>
   </si>
@@ -2998,6 +3027,18 @@
   </si>
   <si>
     <t>DASHBOARD RESPECTO AL TIEMPO</t>
+  </si>
+  <si>
+    <t>Plataforma</t>
+  </si>
+  <si>
+    <t>AÑO</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>DIA DE LA SEMANA</t>
   </si>
 </sst>
 </file>
@@ -3165,7 +3206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3226,12 +3267,6 @@
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3267,6 +3302,30 @@
     </xf>
     <xf numFmtId="17" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6901,9 +6960,94 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v2.15</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.17</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Total</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1" compatLnSpc="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Total</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="funnel" uniqueId="{B5997448-DF7D-2840-AD74-5FAD71A14E22}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v2.16</cx:f>
+              <cx:v>Total</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="1">
+        <cx:catScaling gapWidth="2.26999998"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="26">
+  <a:schemeClr val="accent6"/>
 </cs:colorStyle>
 </file>
 
@@ -7501,6 +7645,525 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="217">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -12134,6 +12797,89 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Gráfico 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1E0112-4AAD-6356-2FC0-D45D0C5E6635}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="101600" y="1479550"/>
+              <a:ext cx="6121400" cy="4057650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-MX" sz="1100"/>
+                <a:t>Este gráfico no está disponible en tu versión de Excel.
+Si editas esta forma o guardas el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -16986,7 +17732,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0135FD6A-8A41-8148-92DE-5B5D8E79EFC8}" name="TablaDinámica2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
   <location ref="F3:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -17175,7 +17921,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C14A41-D46B-BB42-9BF6-EF5715AC2855}" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year_view">
   <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -17319,7 +18065,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA57FC47-D71D-8147-A4A1-59238F532039}" name="TablaDinámica4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
   <location ref="M3:O14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -17527,7 +18273,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4662B47-2F44-4C42-A0F4-4400B73DD201}" name="TablaDinámica3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
   <location ref="J3:K14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -18267,8 +19013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE35869-4E62-4D4B-8B4A-6A1A41B2E18E}">
   <dimension ref="A1:O345"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A312" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F341" sqref="F341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35941,12 +36687,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="36" t="s">
         <v>899</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -36417,16 +37163,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="37" t="s">
         <v>934</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:11" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
@@ -36729,14 +37475,14 @@
       <c r="H14" s="16"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="37" t="s">
         <v>936</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
     </row>
@@ -37197,1225 +37943,1225 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33442D54-C95E-2C4B-BB29-A489FD011890}">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="12" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="26"/>
-    <col min="5" max="5" width="12.6640625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="13" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="26"/>
-    <col min="8" max="8" width="16.83203125" style="26" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="26"/>
+    <col min="1" max="1" width="13.33203125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="24" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="24"/>
+    <col min="5" max="5" width="12.6640625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="13" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="24"/>
+    <col min="8" max="8" width="16.83203125" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
         <v>969</v>
       </c>
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-    </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="22" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="23" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+    </row>
+    <row r="3" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="31" t="s">
         <v>906</v>
       </c>
-      <c r="B58" s="33" t="s">
+      <c r="B58" s="31" t="s">
         <v>943</v>
       </c>
-      <c r="C58" s="33" t="s">
+      <c r="C58" s="31" t="s">
         <v>944</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="D58" s="31" t="s">
         <v>904</v>
       </c>
-      <c r="E58" s="34" t="s">
+      <c r="E58" s="32" t="s">
         <v>945</v>
       </c>
-      <c r="F58" s="33" t="s">
+      <c r="F58" s="31" t="s">
         <v>958</v>
       </c>
-      <c r="G58" s="33" t="s">
+      <c r="G58" s="31" t="s">
         <v>905</v>
       </c>
-      <c r="H58" s="34" t="s">
+      <c r="H58" s="32" t="s">
         <v>959</v>
       </c>
-      <c r="I58" s="33" t="s">
+      <c r="I58" s="31" t="s">
         <v>967</v>
       </c>
-      <c r="J58" s="33" t="s">
+      <c r="J58" s="31" t="s">
         <v>967</v>
       </c>
-      <c r="K58" s="34" t="s">
+      <c r="K58" s="32" t="s">
         <v>968</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="35">
+      <c r="A59" s="33">
         <v>2020</v>
       </c>
-      <c r="B59" s="35">
+      <c r="B59" s="33">
         <f>COUNTIF(Movies!D:D,$A59)</f>
         <v>84</v>
       </c>
-      <c r="C59" s="35">
+      <c r="C59" s="33">
         <v>1</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D59" s="33" t="s">
         <v>946</v>
       </c>
-      <c r="E59" s="35">
+      <c r="E59" s="33">
         <f>COUNTIF(Movies!E:E,$C59)</f>
         <v>45</v>
       </c>
-      <c r="F59" s="35">
+      <c r="F59" s="33">
         <v>1</v>
       </c>
-      <c r="G59" s="35" t="s">
+      <c r="G59" s="33" t="s">
         <v>960</v>
       </c>
-      <c r="H59" s="35">
+      <c r="H59" s="33">
         <f>COUNTIF(Movies!F:F,$F59)</f>
         <v>48</v>
       </c>
-      <c r="I59" s="36">
+      <c r="I59" s="34">
         <v>202001</v>
       </c>
-      <c r="J59" s="37">
+      <c r="J59" s="35">
         <v>43831</v>
       </c>
-      <c r="K59" s="35">
+      <c r="K59" s="33">
         <f>COUNTIF(Movies!C:C,$I59)</f>
         <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="35">
+      <c r="A60" s="33">
         <v>2021</v>
       </c>
-      <c r="B60" s="35">
+      <c r="B60" s="33">
         <f>COUNTIF(Movies!D:D,$A60)</f>
         <v>135</v>
       </c>
-      <c r="C60" s="35">
+      <c r="C60" s="33">
         <v>2</v>
       </c>
-      <c r="D60" s="35" t="s">
+      <c r="D60" s="33" t="s">
         <v>947</v>
       </c>
-      <c r="E60" s="35">
+      <c r="E60" s="33">
         <f>COUNTIF(Movies!E:E,$C60)</f>
         <v>31</v>
       </c>
-      <c r="F60" s="35">
+      <c r="F60" s="33">
         <v>2</v>
       </c>
-      <c r="G60" s="35" t="s">
+      <c r="G60" s="33" t="s">
         <v>961</v>
       </c>
-      <c r="H60" s="35">
+      <c r="H60" s="33">
         <f>COUNTIF(Movies!F:F,$F60)</f>
         <v>28</v>
       </c>
-      <c r="I60" s="36">
+      <c r="I60" s="34">
         <v>202002</v>
       </c>
-      <c r="J60" s="37">
+      <c r="J60" s="35">
         <v>43862</v>
       </c>
-      <c r="K60" s="35">
+      <c r="K60" s="33">
         <f>COUNTIF(Movies!C:C,$I60)</f>
         <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" s="35">
+      <c r="A61" s="33">
         <v>2022</v>
       </c>
-      <c r="B61" s="35">
+      <c r="B61" s="33">
         <f>COUNTIF(Movies!D:D,$A61)</f>
         <v>90</v>
       </c>
-      <c r="C61" s="35">
+      <c r="C61" s="33">
         <v>3</v>
       </c>
-      <c r="D61" s="35" t="s">
+      <c r="D61" s="33" t="s">
         <v>948</v>
       </c>
-      <c r="E61" s="35">
+      <c r="E61" s="33">
         <f>COUNTIF(Movies!E:E,$C61)</f>
         <v>32</v>
       </c>
-      <c r="F61" s="35">
+      <c r="F61" s="33">
         <v>3</v>
       </c>
-      <c r="G61" s="35" t="s">
+      <c r="G61" s="33" t="s">
         <v>962</v>
       </c>
-      <c r="H61" s="35">
+      <c r="H61" s="33">
         <f>COUNTIF(Movies!F:F,$F61)</f>
         <v>33</v>
       </c>
-      <c r="I61" s="36">
+      <c r="I61" s="34">
         <v>202003</v>
       </c>
-      <c r="J61" s="37">
+      <c r="J61" s="35">
         <v>43891</v>
       </c>
-      <c r="K61" s="35">
+      <c r="K61" s="33">
         <f>COUNTIF(Movies!C:C,$I61)</f>
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" s="35">
+      <c r="A62" s="33">
         <v>2023</v>
       </c>
-      <c r="B62" s="35">
+      <c r="B62" s="33">
         <f>COUNTIF(Movies!D:D,$A62)</f>
         <v>35</v>
       </c>
-      <c r="C62" s="35">
+      <c r="C62" s="33">
         <v>4</v>
       </c>
-      <c r="D62" s="35" t="s">
+      <c r="D62" s="33" t="s">
         <v>949</v>
       </c>
-      <c r="E62" s="35">
+      <c r="E62" s="33">
         <f>COUNTIF(Movies!E:E,$C62)</f>
         <v>54</v>
       </c>
-      <c r="F62" s="35">
+      <c r="F62" s="33">
         <v>4</v>
       </c>
-      <c r="G62" s="35" t="s">
+      <c r="G62" s="33" t="s">
         <v>963</v>
       </c>
-      <c r="H62" s="35">
+      <c r="H62" s="33">
         <f>COUNTIF(Movies!F:F,$F62)</f>
         <v>60</v>
       </c>
-      <c r="I62" s="36">
+      <c r="I62" s="34">
         <v>202004</v>
       </c>
-      <c r="J62" s="37">
+      <c r="J62" s="35">
         <v>43922</v>
       </c>
-      <c r="K62" s="35">
+      <c r="K62" s="33">
         <f>COUNTIF(Movies!C:C,$I62)</f>
         <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="35"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35">
+      <c r="A63" s="33"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="33">
         <v>5</v>
       </c>
-      <c r="D63" s="35" t="s">
+      <c r="D63" s="33" t="s">
         <v>950</v>
       </c>
-      <c r="E63" s="35">
+      <c r="E63" s="33">
         <f>COUNTIF(Movies!E:E,$C63)</f>
         <v>38</v>
       </c>
-      <c r="F63" s="35">
+      <c r="F63" s="33">
         <v>5</v>
       </c>
-      <c r="G63" s="35" t="s">
+      <c r="G63" s="33" t="s">
         <v>964</v>
       </c>
-      <c r="H63" s="35">
+      <c r="H63" s="33">
         <f>COUNTIF(Movies!F:F,$F63)</f>
         <v>26</v>
       </c>
-      <c r="I63" s="36">
+      <c r="I63" s="34">
         <v>202005</v>
       </c>
-      <c r="J63" s="37">
+      <c r="J63" s="35">
         <v>43952</v>
       </c>
-      <c r="K63" s="35">
+      <c r="K63" s="33">
         <f>COUNTIF(Movies!C:C,$I63)</f>
         <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="35"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="35">
+      <c r="A64" s="33"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33">
         <v>6</v>
       </c>
-      <c r="D64" s="35" t="s">
+      <c r="D64" s="33" t="s">
         <v>951</v>
       </c>
-      <c r="E64" s="35">
+      <c r="E64" s="33">
         <f>COUNTIF(Movies!E:E,$C64)</f>
         <v>27</v>
       </c>
-      <c r="F64" s="35">
+      <c r="F64" s="33">
         <v>6</v>
       </c>
-      <c r="G64" s="35" t="s">
+      <c r="G64" s="33" t="s">
         <v>965</v>
       </c>
-      <c r="H64" s="35">
+      <c r="H64" s="33">
         <f>COUNTIF(Movies!F:F,$F64)</f>
         <v>67</v>
       </c>
-      <c r="I64" s="36">
+      <c r="I64" s="34">
         <v>202006</v>
       </c>
-      <c r="J64" s="37">
+      <c r="J64" s="35">
         <v>43983</v>
       </c>
-      <c r="K64" s="35">
+      <c r="K64" s="33">
         <f>COUNTIF(Movies!C:C,$I64)</f>
         <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="35"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="35">
+      <c r="A65" s="33"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33">
         <v>7</v>
       </c>
-      <c r="D65" s="35" t="s">
+      <c r="D65" s="33" t="s">
         <v>952</v>
       </c>
-      <c r="E65" s="35">
+      <c r="E65" s="33">
         <f>COUNTIF(Movies!E:E,$C65)</f>
         <v>26</v>
       </c>
-      <c r="F65" s="35">
+      <c r="F65" s="33">
         <v>7</v>
       </c>
-      <c r="G65" s="35" t="s">
+      <c r="G65" s="33" t="s">
         <v>966</v>
       </c>
-      <c r="H65" s="35">
+      <c r="H65" s="33">
         <f>COUNTIF(Movies!F:F,$F65)</f>
         <v>82</v>
       </c>
-      <c r="I65" s="36">
+      <c r="I65" s="34">
         <v>202007</v>
       </c>
-      <c r="J65" s="37">
+      <c r="J65" s="35">
         <v>44013</v>
       </c>
-      <c r="K65" s="35">
+      <c r="K65" s="33">
         <f>COUNTIF(Movies!C:C,$I65)</f>
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" s="35"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="35">
+      <c r="A66" s="33"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33">
         <v>8</v>
       </c>
-      <c r="D66" s="35" t="s">
+      <c r="D66" s="33" t="s">
         <v>953</v>
       </c>
-      <c r="E66" s="35">
+      <c r="E66" s="33">
         <f>COUNTIF(Movies!E:E,$C66)</f>
         <v>22</v>
       </c>
-      <c r="F66" s="35"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="36">
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="34">
         <v>202008</v>
       </c>
-      <c r="J66" s="37">
+      <c r="J66" s="35">
         <v>44044</v>
       </c>
-      <c r="K66" s="35">
+      <c r="K66" s="33">
         <f>COUNTIF(Movies!C:C,$I66)</f>
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35">
+      <c r="A67" s="33"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="33">
         <v>9</v>
       </c>
-      <c r="D67" s="35" t="s">
+      <c r="D67" s="33" t="s">
         <v>954</v>
       </c>
-      <c r="E67" s="35">
+      <c r="E67" s="33">
         <f>COUNTIF(Movies!E:E,$C67)</f>
         <v>17</v>
       </c>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="36">
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="34">
         <v>202009</v>
       </c>
-      <c r="J67" s="37">
+      <c r="J67" s="35">
         <v>44075</v>
       </c>
-      <c r="K67" s="35">
+      <c r="K67" s="33">
         <f>COUNTIF(Movies!C:C,$I67)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" s="35"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35">
+      <c r="A68" s="33"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33">
         <v>10</v>
       </c>
-      <c r="D68" s="35" t="s">
+      <c r="D68" s="33" t="s">
         <v>955</v>
       </c>
-      <c r="E68" s="35">
+      <c r="E68" s="33">
         <f>COUNTIF(Movies!E:E,$C68)</f>
         <v>18</v>
       </c>
-      <c r="F68" s="35"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="35"/>
-      <c r="I68" s="36">
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="34">
         <v>202010</v>
       </c>
-      <c r="J68" s="37">
+      <c r="J68" s="35">
         <v>44105</v>
       </c>
-      <c r="K68" s="35">
+      <c r="K68" s="33">
         <f>COUNTIF(Movies!C:C,$I68)</f>
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="35"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="35">
+      <c r="A69" s="33"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33">
         <v>11</v>
       </c>
-      <c r="D69" s="35" t="s">
+      <c r="D69" s="33" t="s">
         <v>956</v>
       </c>
-      <c r="E69" s="35">
+      <c r="E69" s="33">
         <f>COUNTIF(Movies!E:E,$C69)</f>
         <v>14</v>
       </c>
-      <c r="F69" s="35"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="35"/>
-      <c r="I69" s="36">
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="33"/>
+      <c r="I69" s="34">
         <v>202011</v>
       </c>
-      <c r="J69" s="37">
+      <c r="J69" s="35">
         <v>44136</v>
       </c>
-      <c r="K69" s="35">
+      <c r="K69" s="33">
         <f>COUNTIF(Movies!C:C,$I69)</f>
         <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="35"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35">
+      <c r="A70" s="33"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="33">
         <v>12</v>
       </c>
-      <c r="D70" s="35" t="s">
+      <c r="D70" s="33" t="s">
         <v>957</v>
       </c>
-      <c r="E70" s="35">
+      <c r="E70" s="33">
         <f>COUNTIF(Movies!E:E,$C70)</f>
         <v>20</v>
       </c>
-      <c r="F70" s="35"/>
-      <c r="G70" s="35"/>
-      <c r="H70" s="35"/>
-      <c r="I70" s="36">
+      <c r="F70" s="33"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="33"/>
+      <c r="I70" s="34">
         <v>202012</v>
       </c>
-      <c r="J70" s="37">
+      <c r="J70" s="35">
         <v>44166</v>
       </c>
-      <c r="K70" s="35">
+      <c r="K70" s="33">
         <f>COUNTIF(Movies!C:C,$I70)</f>
         <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="35"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="36">
+      <c r="A71" s="33"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="33"/>
+      <c r="H71" s="33"/>
+      <c r="I71" s="34">
         <v>202101</v>
       </c>
-      <c r="J71" s="37">
+      <c r="J71" s="35">
         <v>44197</v>
       </c>
-      <c r="K71" s="35">
+      <c r="K71" s="33">
         <f>COUNTIF(Movies!C:C,$I71)</f>
         <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="35"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="35"/>
-      <c r="H72" s="35"/>
-      <c r="I72" s="36">
+      <c r="A72" s="33"/>
+      <c r="B72" s="33"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="33"/>
+      <c r="I72" s="34">
         <v>202102</v>
       </c>
-      <c r="J72" s="37">
+      <c r="J72" s="35">
         <v>44228</v>
       </c>
-      <c r="K72" s="35">
+      <c r="K72" s="33">
         <f>COUNTIF(Movies!C:C,$I72)</f>
         <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="35"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="35"/>
-      <c r="H73" s="35"/>
-      <c r="I73" s="36">
+      <c r="A73" s="33"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="34">
         <v>202103</v>
       </c>
-      <c r="J73" s="37">
+      <c r="J73" s="35">
         <v>44256</v>
       </c>
-      <c r="K73" s="35">
+      <c r="K73" s="33">
         <f>COUNTIF(Movies!C:C,$I73)</f>
         <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="35"/>
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="35"/>
-      <c r="H74" s="35"/>
-      <c r="I74" s="36">
+      <c r="A74" s="33"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="34">
         <v>202104</v>
       </c>
-      <c r="J74" s="37">
+      <c r="J74" s="35">
         <v>44287</v>
       </c>
-      <c r="K74" s="35">
+      <c r="K74" s="33">
         <f>COUNTIF(Movies!C:C,$I74)</f>
         <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="35"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="35"/>
-      <c r="I75" s="36">
+      <c r="A75" s="33"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="33"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="33"/>
+      <c r="I75" s="34">
         <v>202105</v>
       </c>
-      <c r="J75" s="37">
+      <c r="J75" s="35">
         <v>44317</v>
       </c>
-      <c r="K75" s="35">
+      <c r="K75" s="33">
         <f>COUNTIF(Movies!C:C,$I75)</f>
         <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="35"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="35"/>
-      <c r="G76" s="35"/>
-      <c r="H76" s="35"/>
-      <c r="I76" s="36">
+      <c r="A76" s="33"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="33"/>
+      <c r="I76" s="34">
         <v>202106</v>
       </c>
-      <c r="J76" s="37">
+      <c r="J76" s="35">
         <v>44348</v>
       </c>
-      <c r="K76" s="35">
+      <c r="K76" s="33">
         <f>COUNTIF(Movies!C:C,$I76)</f>
         <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="35"/>
-      <c r="B77" s="35"/>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="35"/>
-      <c r="H77" s="35"/>
-      <c r="I77" s="36">
+      <c r="A77" s="33"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="33"/>
+      <c r="I77" s="34">
         <v>202107</v>
       </c>
-      <c r="J77" s="37">
+      <c r="J77" s="35">
         <v>44378</v>
       </c>
-      <c r="K77" s="35">
+      <c r="K77" s="33">
         <f>COUNTIF(Movies!C:C,$I77)</f>
         <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="35"/>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="35"/>
-      <c r="G78" s="35"/>
-      <c r="H78" s="35"/>
-      <c r="I78" s="36">
+      <c r="A78" s="33"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="33"/>
+      <c r="I78" s="34">
         <v>202108</v>
       </c>
-      <c r="J78" s="37">
+      <c r="J78" s="35">
         <v>44409</v>
       </c>
-      <c r="K78" s="35">
+      <c r="K78" s="33">
         <f>COUNTIF(Movies!C:C,$I78)</f>
         <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="35"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="35"/>
-      <c r="H79" s="35"/>
-      <c r="I79" s="36">
+      <c r="A79" s="33"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="33"/>
+      <c r="D79" s="33"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="33"/>
+      <c r="I79" s="34">
         <v>202109</v>
       </c>
-      <c r="J79" s="37">
+      <c r="J79" s="35">
         <v>44440</v>
       </c>
-      <c r="K79" s="35">
+      <c r="K79" s="33">
         <f>COUNTIF(Movies!C:C,$I79)</f>
         <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="35"/>
-      <c r="B80" s="35"/>
-      <c r="C80" s="35"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="35"/>
-      <c r="H80" s="35"/>
-      <c r="I80" s="36">
+      <c r="A80" s="33"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="33"/>
+      <c r="I80" s="34">
         <v>202110</v>
       </c>
-      <c r="J80" s="37">
+      <c r="J80" s="35">
         <v>44470</v>
       </c>
-      <c r="K80" s="35">
+      <c r="K80" s="33">
         <f>COUNTIF(Movies!C:C,$I80)</f>
         <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="35"/>
-      <c r="B81" s="35"/>
-      <c r="C81" s="35"/>
-      <c r="D81" s="35"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="35"/>
-      <c r="H81" s="35"/>
-      <c r="I81" s="36">
+      <c r="A81" s="33"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="33"/>
+      <c r="E81" s="33"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="33"/>
+      <c r="I81" s="34">
         <v>202111</v>
       </c>
-      <c r="J81" s="37">
+      <c r="J81" s="35">
         <v>44501</v>
       </c>
-      <c r="K81" s="35">
+      <c r="K81" s="33">
         <f>COUNTIF(Movies!C:C,$I81)</f>
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="35"/>
-      <c r="B82" s="35"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="35"/>
-      <c r="H82" s="35"/>
-      <c r="I82" s="36">
+      <c r="A82" s="33"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+      <c r="H82" s="33"/>
+      <c r="I82" s="34">
         <v>202112</v>
       </c>
-      <c r="J82" s="37">
+      <c r="J82" s="35">
         <v>44531</v>
       </c>
-      <c r="K82" s="35">
+      <c r="K82" s="33">
         <f>COUNTIF(Movies!C:C,$I82)</f>
         <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="35"/>
-      <c r="B83" s="35"/>
-      <c r="C83" s="35"/>
-      <c r="D83" s="35"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="35"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="35"/>
-      <c r="I83" s="36">
+      <c r="A83" s="33"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="34">
         <v>202201</v>
       </c>
-      <c r="J83" s="37">
+      <c r="J83" s="35">
         <v>44562</v>
       </c>
-      <c r="K83" s="35">
+      <c r="K83" s="33">
         <f>COUNTIF(Movies!C:C,$I83)</f>
         <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" s="35"/>
-      <c r="B84" s="35"/>
-      <c r="C84" s="35"/>
-      <c r="D84" s="35"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="35"/>
-      <c r="G84" s="35"/>
-      <c r="H84" s="35"/>
-      <c r="I84" s="36">
+      <c r="A84" s="33"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="33"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="33"/>
+      <c r="I84" s="34">
         <v>202202</v>
       </c>
-      <c r="J84" s="37">
+      <c r="J84" s="35">
         <v>44593</v>
       </c>
-      <c r="K84" s="35">
+      <c r="K84" s="33">
         <f>COUNTIF(Movies!C:C,$I84)</f>
         <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" s="35"/>
-      <c r="B85" s="35"/>
-      <c r="C85" s="35"/>
-      <c r="D85" s="35"/>
-      <c r="E85" s="35"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="35"/>
-      <c r="H85" s="35"/>
-      <c r="I85" s="36">
+      <c r="A85" s="33"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="33"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="33"/>
+      <c r="I85" s="34">
         <v>202203</v>
       </c>
-      <c r="J85" s="37">
+      <c r="J85" s="35">
         <v>44621</v>
       </c>
-      <c r="K85" s="35">
+      <c r="K85" s="33">
         <f>COUNTIF(Movies!C:C,$I85)</f>
         <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" s="35"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="35"/>
-      <c r="H86" s="35"/>
-      <c r="I86" s="36">
+      <c r="A86" s="33"/>
+      <c r="B86" s="33"/>
+      <c r="C86" s="33"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="33"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="33"/>
+      <c r="H86" s="33"/>
+      <c r="I86" s="34">
         <v>202204</v>
       </c>
-      <c r="J86" s="37">
+      <c r="J86" s="35">
         <v>44652</v>
       </c>
-      <c r="K86" s="35">
+      <c r="K86" s="33">
         <f>COUNTIF(Movies!C:C,$I86)</f>
         <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A87" s="35"/>
-      <c r="B87" s="35"/>
-      <c r="C87" s="35"/>
-      <c r="D87" s="35"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="35"/>
-      <c r="H87" s="35"/>
-      <c r="I87" s="36">
+      <c r="A87" s="33"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="33"/>
+      <c r="G87" s="33"/>
+      <c r="H87" s="33"/>
+      <c r="I87" s="34">
         <v>202205</v>
       </c>
-      <c r="J87" s="37">
+      <c r="J87" s="35">
         <v>44682</v>
       </c>
-      <c r="K87" s="35">
+      <c r="K87" s="33">
         <f>COUNTIF(Movies!C:C,$I87)</f>
         <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" s="35"/>
-      <c r="B88" s="35"/>
-      <c r="C88" s="35"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="35"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="35"/>
-      <c r="H88" s="35"/>
-      <c r="I88" s="36">
+      <c r="A88" s="33"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="I88" s="34">
         <v>202206</v>
       </c>
-      <c r="J88" s="37">
+      <c r="J88" s="35">
         <v>44713</v>
       </c>
-      <c r="K88" s="35">
+      <c r="K88" s="33">
         <f>COUNTIF(Movies!C:C,$I88)</f>
         <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" s="35"/>
-      <c r="B89" s="35"/>
-      <c r="C89" s="35"/>
-      <c r="D89" s="35"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="35"/>
-      <c r="H89" s="35"/>
-      <c r="I89" s="36">
+      <c r="A89" s="33"/>
+      <c r="B89" s="33"/>
+      <c r="C89" s="33"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="33"/>
+      <c r="H89" s="33"/>
+      <c r="I89" s="34">
         <v>202207</v>
       </c>
-      <c r="J89" s="37">
+      <c r="J89" s="35">
         <v>44743</v>
       </c>
-      <c r="K89" s="35">
+      <c r="K89" s="33">
         <f>COUNTIF(Movies!C:C,$I89)</f>
         <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" s="35"/>
-      <c r="B90" s="35"/>
-      <c r="C90" s="35"/>
-      <c r="D90" s="35"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="35"/>
-      <c r="H90" s="35"/>
-      <c r="I90" s="36">
+      <c r="A90" s="33"/>
+      <c r="B90" s="33"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="33"/>
+      <c r="G90" s="33"/>
+      <c r="H90" s="33"/>
+      <c r="I90" s="34">
         <v>202208</v>
       </c>
-      <c r="J90" s="37">
+      <c r="J90" s="35">
         <v>44774</v>
       </c>
-      <c r="K90" s="35">
+      <c r="K90" s="33">
         <f>COUNTIF(Movies!C:C,$I90)</f>
         <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" s="35"/>
-      <c r="B91" s="35"/>
-      <c r="C91" s="35"/>
-      <c r="D91" s="35"/>
-      <c r="E91" s="35"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="35"/>
-      <c r="I91" s="36">
+      <c r="A91" s="33"/>
+      <c r="B91" s="33"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="33"/>
+      <c r="E91" s="33"/>
+      <c r="F91" s="33"/>
+      <c r="G91" s="33"/>
+      <c r="H91" s="33"/>
+      <c r="I91" s="34">
         <v>202209</v>
       </c>
-      <c r="J91" s="37">
+      <c r="J91" s="35">
         <v>44805</v>
       </c>
-      <c r="K91" s="35">
+      <c r="K91" s="33">
         <f>COUNTIF(Movies!C:C,$I91)</f>
         <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" s="35"/>
-      <c r="B92" s="35"/>
-      <c r="C92" s="35"/>
-      <c r="D92" s="35"/>
-      <c r="E92" s="35"/>
-      <c r="F92" s="35"/>
-      <c r="G92" s="35"/>
-      <c r="H92" s="35"/>
-      <c r="I92" s="36">
+      <c r="A92" s="33"/>
+      <c r="B92" s="33"/>
+      <c r="C92" s="33"/>
+      <c r="D92" s="33"/>
+      <c r="E92" s="33"/>
+      <c r="F92" s="33"/>
+      <c r="G92" s="33"/>
+      <c r="H92" s="33"/>
+      <c r="I92" s="34">
         <v>202210</v>
       </c>
-      <c r="J92" s="37">
+      <c r="J92" s="35">
         <v>44835</v>
       </c>
-      <c r="K92" s="35">
+      <c r="K92" s="33">
         <f>COUNTIF(Movies!C:C,$I92)</f>
         <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" s="35"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="35"/>
-      <c r="D93" s="35"/>
-      <c r="E93" s="35"/>
-      <c r="F93" s="35"/>
-      <c r="G93" s="35"/>
-      <c r="H93" s="35"/>
-      <c r="I93" s="36">
+      <c r="A93" s="33"/>
+      <c r="B93" s="33"/>
+      <c r="C93" s="33"/>
+      <c r="D93" s="33"/>
+      <c r="E93" s="33"/>
+      <c r="F93" s="33"/>
+      <c r="G93" s="33"/>
+      <c r="H93" s="33"/>
+      <c r="I93" s="34">
         <v>202211</v>
       </c>
-      <c r="J93" s="37">
+      <c r="J93" s="35">
         <v>44866</v>
       </c>
-      <c r="K93" s="35">
+      <c r="K93" s="33">
         <f>COUNTIF(Movies!C:C,$I93)</f>
         <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="35"/>
-      <c r="B94" s="35"/>
-      <c r="C94" s="35"/>
-      <c r="D94" s="35"/>
-      <c r="E94" s="35"/>
-      <c r="F94" s="35"/>
-      <c r="G94" s="35"/>
-      <c r="H94" s="35"/>
-      <c r="I94" s="36">
+      <c r="A94" s="33"/>
+      <c r="B94" s="33"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="33"/>
+      <c r="F94" s="33"/>
+      <c r="G94" s="33"/>
+      <c r="H94" s="33"/>
+      <c r="I94" s="34">
         <v>202212</v>
       </c>
-      <c r="J94" s="37">
+      <c r="J94" s="35">
         <v>44896</v>
       </c>
-      <c r="K94" s="35">
+      <c r="K94" s="33">
         <f>COUNTIF(Movies!C:C,$I94)</f>
         <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="35"/>
-      <c r="B95" s="35"/>
-      <c r="C95" s="35"/>
-      <c r="D95" s="35"/>
-      <c r="E95" s="35"/>
-      <c r="F95" s="35"/>
-      <c r="G95" s="35"/>
-      <c r="H95" s="35"/>
-      <c r="I95" s="36">
+      <c r="A95" s="33"/>
+      <c r="B95" s="33"/>
+      <c r="C95" s="33"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="33"/>
+      <c r="F95" s="33"/>
+      <c r="G95" s="33"/>
+      <c r="H95" s="33"/>
+      <c r="I95" s="34">
         <v>202301</v>
       </c>
-      <c r="J95" s="37">
+      <c r="J95" s="35">
         <v>44927</v>
       </c>
-      <c r="K95" s="35">
+      <c r="K95" s="33">
         <f>COUNTIF(Movies!C:C,$I95)</f>
         <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" s="35"/>
-      <c r="B96" s="35"/>
-      <c r="C96" s="35"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="35"/>
-      <c r="G96" s="35"/>
-      <c r="H96" s="35"/>
-      <c r="I96" s="36">
+      <c r="A96" s="33"/>
+      <c r="B96" s="33"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33"/>
+      <c r="G96" s="33"/>
+      <c r="H96" s="33"/>
+      <c r="I96" s="34">
         <v>202302</v>
       </c>
-      <c r="J96" s="37">
+      <c r="J96" s="35">
         <v>44958</v>
       </c>
-      <c r="K96" s="35">
+      <c r="K96" s="33">
         <f>COUNTIF(Movies!C:C,$I96)</f>
         <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A97" s="35"/>
-      <c r="B97" s="35"/>
-      <c r="C97" s="35"/>
-      <c r="D97" s="35"/>
-      <c r="E97" s="35"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="35"/>
-      <c r="H97" s="35"/>
-      <c r="I97" s="36">
+      <c r="A97" s="33"/>
+      <c r="B97" s="33"/>
+      <c r="C97" s="33"/>
+      <c r="D97" s="33"/>
+      <c r="E97" s="33"/>
+      <c r="F97" s="33"/>
+      <c r="G97" s="33"/>
+      <c r="H97" s="33"/>
+      <c r="I97" s="34">
         <v>202303</v>
       </c>
-      <c r="J97" s="37">
+      <c r="J97" s="35">
         <v>44986</v>
       </c>
-      <c r="K97" s="35">
+      <c r="K97" s="33">
         <f>COUNTIF(Movies!C:C,$I97)</f>
         <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="35"/>
-      <c r="B98" s="35"/>
-      <c r="C98" s="35"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="35"/>
-      <c r="H98" s="35"/>
-      <c r="I98" s="36">
+      <c r="A98" s="33"/>
+      <c r="B98" s="33"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="33"/>
+      <c r="G98" s="33"/>
+      <c r="H98" s="33"/>
+      <c r="I98" s="34">
         <v>202304</v>
       </c>
-      <c r="J98" s="37">
+      <c r="J98" s="35">
         <v>45017</v>
       </c>
-      <c r="K98" s="35">
+      <c r="K98" s="33">
         <f>COUNTIF(Movies!C:C,$I98)</f>
         <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A99" s="35"/>
-      <c r="B99" s="35"/>
-      <c r="C99" s="35"/>
-      <c r="D99" s="35"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="35"/>
-      <c r="G99" s="35"/>
-      <c r="H99" s="35"/>
-      <c r="I99" s="36">
+      <c r="A99" s="33"/>
+      <c r="B99" s="33"/>
+      <c r="C99" s="33"/>
+      <c r="D99" s="33"/>
+      <c r="E99" s="33"/>
+      <c r="F99" s="33"/>
+      <c r="G99" s="33"/>
+      <c r="H99" s="33"/>
+      <c r="I99" s="34">
         <v>202305</v>
       </c>
-      <c r="J99" s="37">
+      <c r="J99" s="35">
         <v>45047</v>
       </c>
-      <c r="K99" s="35">
+      <c r="K99" s="33">
         <f>COUNTIF(Movies!C:C,$I99)</f>
         <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100" s="35"/>
-      <c r="B100" s="35"/>
-      <c r="C100" s="35"/>
-      <c r="D100" s="35"/>
-      <c r="E100" s="35"/>
-      <c r="F100" s="35"/>
-      <c r="G100" s="35"/>
-      <c r="H100" s="35"/>
-      <c r="I100" s="36">
+      <c r="A100" s="33"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="33"/>
+      <c r="G100" s="33"/>
+      <c r="H100" s="33"/>
+      <c r="I100" s="34">
         <v>202306</v>
       </c>
-      <c r="J100" s="37">
+      <c r="J100" s="35">
         <v>45078</v>
       </c>
-      <c r="K100" s="35">
+      <c r="K100" s="33">
         <f>COUNTIF(Movies!C:C,$I100)</f>
         <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" s="35"/>
-      <c r="B101" s="35"/>
-      <c r="C101" s="35"/>
-      <c r="D101" s="35"/>
-      <c r="E101" s="35"/>
-      <c r="F101" s="35"/>
-      <c r="G101" s="35"/>
-      <c r="H101" s="35"/>
-      <c r="I101" s="36">
+      <c r="A101" s="33"/>
+      <c r="B101" s="33"/>
+      <c r="C101" s="33"/>
+      <c r="D101" s="33"/>
+      <c r="E101" s="33"/>
+      <c r="F101" s="33"/>
+      <c r="G101" s="33"/>
+      <c r="H101" s="33"/>
+      <c r="I101" s="34">
         <v>202307</v>
       </c>
-      <c r="J101" s="37">
+      <c r="J101" s="35">
         <v>45108</v>
       </c>
-      <c r="K101" s="35">
+      <c r="K101" s="33">
         <f>COUNTIF(Movies!C:C,$I101)</f>
         <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A102" s="35"/>
-      <c r="B102" s="35"/>
-      <c r="C102" s="35"/>
-      <c r="D102" s="35"/>
-      <c r="E102" s="35"/>
-      <c r="F102" s="35"/>
-      <c r="G102" s="35"/>
-      <c r="H102" s="35"/>
-      <c r="I102" s="36">
+      <c r="A102" s="33"/>
+      <c r="B102" s="33"/>
+      <c r="C102" s="33"/>
+      <c r="D102" s="33"/>
+      <c r="E102" s="33"/>
+      <c r="F102" s="33"/>
+      <c r="G102" s="33"/>
+      <c r="H102" s="33"/>
+      <c r="I102" s="34">
         <v>202308</v>
       </c>
-      <c r="J102" s="37">
+      <c r="J102" s="35">
         <v>45139</v>
       </c>
-      <c r="K102" s="35">
+      <c r="K102" s="33">
         <f>COUNTIF(Movies!C:C,$I102)</f>
         <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A103" s="35"/>
-      <c r="B103" s="35"/>
-      <c r="C103" s="35"/>
-      <c r="D103" s="35"/>
-      <c r="E103" s="35"/>
-      <c r="F103" s="35"/>
-      <c r="G103" s="35"/>
-      <c r="H103" s="35"/>
-      <c r="I103" s="36">
+      <c r="A103" s="33"/>
+      <c r="B103" s="33"/>
+      <c r="C103" s="33"/>
+      <c r="D103" s="33"/>
+      <c r="E103" s="33"/>
+      <c r="F103" s="33"/>
+      <c r="G103" s="33"/>
+      <c r="H103" s="33"/>
+      <c r="I103" s="34">
         <v>202309</v>
       </c>
-      <c r="J103" s="37">
+      <c r="J103" s="35">
         <v>45170</v>
       </c>
-      <c r="K103" s="35">
+      <c r="K103" s="33">
         <f>COUNTIF(Movies!C:C,$I103)</f>
         <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A104" s="35"/>
-      <c r="B104" s="35"/>
-      <c r="C104" s="35"/>
-      <c r="D104" s="35"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="35"/>
-      <c r="H104" s="35"/>
-      <c r="I104" s="36">
+      <c r="A104" s="33"/>
+      <c r="B104" s="33"/>
+      <c r="C104" s="33"/>
+      <c r="D104" s="33"/>
+      <c r="E104" s="33"/>
+      <c r="F104" s="33"/>
+      <c r="G104" s="33"/>
+      <c r="H104" s="33"/>
+      <c r="I104" s="34">
         <v>202310</v>
       </c>
-      <c r="J104" s="37">
+      <c r="J104" s="35">
         <v>45200</v>
       </c>
-      <c r="K104" s="35">
+      <c r="K104" s="33">
         <f>COUNTIF(Movies!C:C,$I104)</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" s="35"/>
-      <c r="B105" s="35"/>
-      <c r="C105" s="35"/>
-      <c r="D105" s="35"/>
-      <c r="E105" s="35"/>
-      <c r="F105" s="35"/>
-      <c r="G105" s="35"/>
-      <c r="H105" s="35"/>
-      <c r="I105" s="36">
+      <c r="A105" s="33"/>
+      <c r="B105" s="33"/>
+      <c r="C105" s="33"/>
+      <c r="D105" s="33"/>
+      <c r="E105" s="33"/>
+      <c r="F105" s="33"/>
+      <c r="G105" s="33"/>
+      <c r="H105" s="33"/>
+      <c r="I105" s="34">
         <v>202311</v>
       </c>
-      <c r="J105" s="37">
+      <c r="J105" s="35">
         <v>45231</v>
       </c>
-      <c r="K105" s="35">
+      <c r="K105" s="33">
         <f>COUNTIF(Movies!C:C,$I105)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A106" s="35"/>
-      <c r="B106" s="35"/>
-      <c r="C106" s="35"/>
-      <c r="D106" s="35"/>
-      <c r="E106" s="35"/>
-      <c r="F106" s="35"/>
-      <c r="G106" s="35"/>
-      <c r="H106" s="35"/>
-      <c r="I106" s="36">
+      <c r="A106" s="33"/>
+      <c r="B106" s="33"/>
+      <c r="C106" s="33"/>
+      <c r="D106" s="33"/>
+      <c r="E106" s="33"/>
+      <c r="F106" s="33"/>
+      <c r="G106" s="33"/>
+      <c r="H106" s="33"/>
+      <c r="I106" s="34">
         <v>202312</v>
       </c>
-      <c r="J106" s="37">
+      <c r="J106" s="35">
         <v>45261</v>
       </c>
-      <c r="K106" s="35">
+      <c r="K106" s="33">
         <f>COUNTIF(Movies!C:C,$I106)</f>
         <v>0</v>
       </c>
@@ -38425,4 +39171,1991 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697C66FA-5853-064A-AE68-E03A2E58241B}">
+  <dimension ref="A1:Y43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B1" s="38"/>
+      <c r="C1" s="43" t="s">
+        <v>971</v>
+      </c>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43" t="s">
+        <v>972</v>
+      </c>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="37" t="s">
+        <v>973</v>
+      </c>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C2" s="42">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="42">
+        <v>2021</v>
+      </c>
+      <c r="E2" s="42">
+        <v>2022</v>
+      </c>
+      <c r="F2" s="42">
+        <v>2023</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>946</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>947</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>948</v>
+      </c>
+      <c r="J2" s="42" t="s">
+        <v>949</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>950</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>951</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>952</v>
+      </c>
+      <c r="N2" s="42" t="s">
+        <v>953</v>
+      </c>
+      <c r="O2" s="42" t="s">
+        <v>954</v>
+      </c>
+      <c r="P2" s="42" t="s">
+        <v>955</v>
+      </c>
+      <c r="Q2" s="42" t="s">
+        <v>956</v>
+      </c>
+      <c r="R2" s="42" t="s">
+        <v>957</v>
+      </c>
+      <c r="S2" s="42" t="s">
+        <v>960</v>
+      </c>
+      <c r="T2" s="42" t="s">
+        <v>961</v>
+      </c>
+      <c r="U2" s="42" t="s">
+        <v>962</v>
+      </c>
+      <c r="V2" s="42" t="s">
+        <v>963</v>
+      </c>
+      <c r="W2" s="42" t="s">
+        <v>964</v>
+      </c>
+      <c r="X2" s="42" t="s">
+        <v>965</v>
+      </c>
+      <c r="Y2" s="42" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>937</v>
+      </c>
+      <c r="C3" s="42">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="42">
+        <v>2021</v>
+      </c>
+      <c r="E3" s="42">
+        <v>2022</v>
+      </c>
+      <c r="F3" s="42">
+        <v>2023</v>
+      </c>
+      <c r="G3" s="38">
+        <v>1</v>
+      </c>
+      <c r="H3" s="38">
+        <v>2</v>
+      </c>
+      <c r="I3" s="38">
+        <v>3</v>
+      </c>
+      <c r="J3" s="38">
+        <v>4</v>
+      </c>
+      <c r="K3" s="38">
+        <v>5</v>
+      </c>
+      <c r="L3" s="38">
+        <v>6</v>
+      </c>
+      <c r="M3" s="38">
+        <v>7</v>
+      </c>
+      <c r="N3" s="38">
+        <v>8</v>
+      </c>
+      <c r="O3" s="38">
+        <v>9</v>
+      </c>
+      <c r="P3" s="38">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="38">
+        <v>11</v>
+      </c>
+      <c r="R3" s="38">
+        <v>12</v>
+      </c>
+      <c r="S3" s="38">
+        <v>1</v>
+      </c>
+      <c r="T3" s="38">
+        <v>2</v>
+      </c>
+      <c r="U3" s="38">
+        <v>3</v>
+      </c>
+      <c r="V3" s="38">
+        <v>4</v>
+      </c>
+      <c r="W3" s="38">
+        <v>5</v>
+      </c>
+      <c r="X3" s="38">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>660</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIF(Movies!$L:$L,$A4)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>1</v>
+      </c>
+      <c r="X4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A4,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIF(Movies!$L:$L,$A5)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>1</v>
+      </c>
+      <c r="T5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A5,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIF(Movies!$L:$L,$A6)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>1</v>
+      </c>
+      <c r="T6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A6,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>577</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIF(Movies!$L:$L,$A7)</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>2</v>
+      </c>
+      <c r="S7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>1</v>
+      </c>
+      <c r="U7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>1</v>
+      </c>
+      <c r="W7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A7,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>569</v>
+      </c>
+      <c r="B8">
+        <f>COUNTIF(Movies!$L:$L,$A8)</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>1</v>
+      </c>
+      <c r="O8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>1</v>
+      </c>
+      <c r="S8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>1</v>
+      </c>
+      <c r="W8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>0</v>
+      </c>
+      <c r="X8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A8,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>604</v>
+      </c>
+      <c r="B9">
+        <f>COUNTIF(Movies!$L:$L,$A9)</f>
+        <v>3</v>
+      </c>
+      <c r="C9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>2</v>
+      </c>
+      <c r="K9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>1</v>
+      </c>
+      <c r="W9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>1</v>
+      </c>
+      <c r="Y9" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A9,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>591</v>
+      </c>
+      <c r="B10">
+        <f>COUNTIF(Movies!$L:$L,$A10)</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>2</v>
+      </c>
+      <c r="H10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>1</v>
+      </c>
+      <c r="M10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>1</v>
+      </c>
+      <c r="T10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>1</v>
+      </c>
+      <c r="V10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>1</v>
+      </c>
+      <c r="Y10" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A10,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>492</v>
+      </c>
+      <c r="B11">
+        <f>COUNTIF(Movies!$L:$L,$A11)</f>
+        <v>11</v>
+      </c>
+      <c r="C11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>3</v>
+      </c>
+      <c r="F11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>4</v>
+      </c>
+      <c r="G11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>1</v>
+      </c>
+      <c r="M11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>1</v>
+      </c>
+      <c r="O11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>1</v>
+      </c>
+      <c r="P11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>3</v>
+      </c>
+      <c r="Q11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>2</v>
+      </c>
+      <c r="R11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>3</v>
+      </c>
+      <c r="T11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>1</v>
+      </c>
+      <c r="V11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>3</v>
+      </c>
+      <c r="W11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>2</v>
+      </c>
+      <c r="Y11" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A11,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12">
+        <f>COUNTIF(Movies!$L:$L,$A12)</f>
+        <v>12</v>
+      </c>
+      <c r="C12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>2</v>
+      </c>
+      <c r="D12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>5</v>
+      </c>
+      <c r="E12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>3</v>
+      </c>
+      <c r="L12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>2</v>
+      </c>
+      <c r="M12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>1</v>
+      </c>
+      <c r="P12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>1</v>
+      </c>
+      <c r="R12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>2</v>
+      </c>
+      <c r="S12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>1</v>
+      </c>
+      <c r="U12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>4</v>
+      </c>
+      <c r="V12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>5</v>
+      </c>
+      <c r="W12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>1</v>
+      </c>
+      <c r="X12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A12,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>314</v>
+      </c>
+      <c r="B13">
+        <f>COUNTIF(Movies!$L:$L,$A13)</f>
+        <v>18</v>
+      </c>
+      <c r="C13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>15</v>
+      </c>
+      <c r="E13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>2</v>
+      </c>
+      <c r="H13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>2</v>
+      </c>
+      <c r="J13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>3</v>
+      </c>
+      <c r="K13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>2</v>
+      </c>
+      <c r="L13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>2</v>
+      </c>
+      <c r="O13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>3</v>
+      </c>
+      <c r="P13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>1</v>
+      </c>
+      <c r="R13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>3</v>
+      </c>
+      <c r="U13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>5</v>
+      </c>
+      <c r="W13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>3</v>
+      </c>
+      <c r="X13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>2</v>
+      </c>
+      <c r="Y13" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A13,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <f>COUNTIF(Movies!$L:$L,$A14)</f>
+        <v>33</v>
+      </c>
+      <c r="C14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>4</v>
+      </c>
+      <c r="D14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>10</v>
+      </c>
+      <c r="E14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>12</v>
+      </c>
+      <c r="F14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>7</v>
+      </c>
+      <c r="G14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>5</v>
+      </c>
+      <c r="H14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>4</v>
+      </c>
+      <c r="I14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>3</v>
+      </c>
+      <c r="J14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>2</v>
+      </c>
+      <c r="K14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>1</v>
+      </c>
+      <c r="L14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>7</v>
+      </c>
+      <c r="M14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>5</v>
+      </c>
+      <c r="N14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>2</v>
+      </c>
+      <c r="O14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>1</v>
+      </c>
+      <c r="P14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>1</v>
+      </c>
+      <c r="R14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>1</v>
+      </c>
+      <c r="S14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>5</v>
+      </c>
+      <c r="U14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>7</v>
+      </c>
+      <c r="V14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>18</v>
+      </c>
+      <c r="W14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>2</v>
+      </c>
+      <c r="X14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>1</v>
+      </c>
+      <c r="Y14" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15">
+        <f>COUNTIF(Movies!$L:$L,$A15)</f>
+        <v>44</v>
+      </c>
+      <c r="C15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>4</v>
+      </c>
+      <c r="D15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>23</v>
+      </c>
+      <c r="E15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>16</v>
+      </c>
+      <c r="F15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>6</v>
+      </c>
+      <c r="H15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>5</v>
+      </c>
+      <c r="I15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>5</v>
+      </c>
+      <c r="J15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>4</v>
+      </c>
+      <c r="K15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>3</v>
+      </c>
+      <c r="L15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>3</v>
+      </c>
+      <c r="M15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>4</v>
+      </c>
+      <c r="N15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>3</v>
+      </c>
+      <c r="O15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>2</v>
+      </c>
+      <c r="P15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>2</v>
+      </c>
+      <c r="Q15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>2</v>
+      </c>
+      <c r="R15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>5</v>
+      </c>
+      <c r="S15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>10</v>
+      </c>
+      <c r="T15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>5</v>
+      </c>
+      <c r="U15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>4</v>
+      </c>
+      <c r="V15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>8</v>
+      </c>
+      <c r="W15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>5</v>
+      </c>
+      <c r="X15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>5</v>
+      </c>
+      <c r="Y15" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A15,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f>COUNTIF(Movies!$L:$L,$A16)</f>
+        <v>67</v>
+      </c>
+      <c r="C16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>16</v>
+      </c>
+      <c r="D16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>26</v>
+      </c>
+      <c r="E16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>18</v>
+      </c>
+      <c r="F16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>7</v>
+      </c>
+      <c r="G16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>9</v>
+      </c>
+      <c r="H16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>7</v>
+      </c>
+      <c r="I16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>5</v>
+      </c>
+      <c r="J16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>12</v>
+      </c>
+      <c r="K16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>9</v>
+      </c>
+      <c r="L16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>3</v>
+      </c>
+      <c r="M16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>5</v>
+      </c>
+      <c r="N16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>4</v>
+      </c>
+      <c r="O16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>3</v>
+      </c>
+      <c r="P16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>5</v>
+      </c>
+      <c r="Q16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>2</v>
+      </c>
+      <c r="R16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>3</v>
+      </c>
+      <c r="S16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>13</v>
+      </c>
+      <c r="T16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>5</v>
+      </c>
+      <c r="U16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>1</v>
+      </c>
+      <c r="V16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>5</v>
+      </c>
+      <c r="W16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>5</v>
+      </c>
+      <c r="X16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>22</v>
+      </c>
+      <c r="Y16" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A16,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <f>COUNTIF(Movies!$L:$L,$A17)</f>
+        <v>71</v>
+      </c>
+      <c r="C17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>28</v>
+      </c>
+      <c r="D17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>24</v>
+      </c>
+      <c r="E17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>15</v>
+      </c>
+      <c r="F17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>6</v>
+      </c>
+      <c r="H17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>4</v>
+      </c>
+      <c r="I17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>7</v>
+      </c>
+      <c r="J17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>19</v>
+      </c>
+      <c r="K17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>10</v>
+      </c>
+      <c r="L17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>5</v>
+      </c>
+      <c r="M17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>5</v>
+      </c>
+      <c r="N17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>5</v>
+      </c>
+      <c r="O17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>2</v>
+      </c>
+      <c r="P17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>2</v>
+      </c>
+      <c r="Q17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>3</v>
+      </c>
+      <c r="R17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>3</v>
+      </c>
+      <c r="S17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>9</v>
+      </c>
+      <c r="T17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>2</v>
+      </c>
+      <c r="U17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>5</v>
+      </c>
+      <c r="V17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>7</v>
+      </c>
+      <c r="W17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>7</v>
+      </c>
+      <c r="X17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>18</v>
+      </c>
+      <c r="Y17" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A17,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f>COUNTIF(Movies!$L:$L,$A18)</f>
+        <v>72</v>
+      </c>
+      <c r="C18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$D:$D,Hoja1!C$3)</f>
+        <v>30</v>
+      </c>
+      <c r="D18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$D:$D,Hoja1!D$3)</f>
+        <v>23</v>
+      </c>
+      <c r="E18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$D:$D,Hoja1!E$3)</f>
+        <v>16</v>
+      </c>
+      <c r="F18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$D:$D,Hoja1!F$3)</f>
+        <v>3</v>
+      </c>
+      <c r="G18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!G$3)</f>
+        <v>10</v>
+      </c>
+      <c r="H18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!H$3)</f>
+        <v>8</v>
+      </c>
+      <c r="I18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!I$3)</f>
+        <v>9</v>
+      </c>
+      <c r="J18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!J$3)</f>
+        <v>10</v>
+      </c>
+      <c r="K18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!K$3)</f>
+        <v>10</v>
+      </c>
+      <c r="L18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!L$3)</f>
+        <v>4</v>
+      </c>
+      <c r="M18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!M$3)</f>
+        <v>5</v>
+      </c>
+      <c r="N18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!N$3)</f>
+        <v>3</v>
+      </c>
+      <c r="O18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!O$3)</f>
+        <v>3</v>
+      </c>
+      <c r="P18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!P$3)</f>
+        <v>5</v>
+      </c>
+      <c r="Q18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!Q$3)</f>
+        <v>2</v>
+      </c>
+      <c r="R18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$E:$E,Hoja1!R$3)</f>
+        <v>3</v>
+      </c>
+      <c r="S18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$F:$F,Hoja1!S$3)</f>
+        <v>10</v>
+      </c>
+      <c r="T18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$F:$F,Hoja1!T$3)</f>
+        <v>6</v>
+      </c>
+      <c r="U18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$F:$F,Hoja1!U$3)</f>
+        <v>10</v>
+      </c>
+      <c r="V18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$F:$F,Hoja1!V$3)</f>
+        <v>6</v>
+      </c>
+      <c r="W18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$F:$F,Hoja1!W$3)</f>
+        <v>2</v>
+      </c>
+      <c r="X18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$F:$F,Hoja1!X$3)</f>
+        <v>15</v>
+      </c>
+      <c r="Y18" s="38">
+        <f>COUNTIFS(Movies!$L:$L,Hoja1!$A18,Movies!$F:$F,Hoja1!Y$3)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="38"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="38"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="38"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="38"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="38"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="38"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="38"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="38"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="38"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="38"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="38"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="38"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="38"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="38"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="38"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="38"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>970</v>
+      </c>
+      <c r="B41" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>906</v>
+      </c>
+      <c r="B42">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>937</v>
+      </c>
+      <c r="B43">
+        <f>INDEX($B$4:$F$18,MATCH(B41,$A$4:$A$18,0),MATCH(B42,$B$3:$F$3,0))</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Y18" xr:uid="{697C66FA-5853-064A-AE68-E03A2E58241B}">
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+    <filterColumn colId="4" showButton="0"/>
+    <filterColumn colId="6" showButton="0"/>
+    <filterColumn colId="7" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="10" showButton="0"/>
+    <filterColumn colId="11" showButton="0"/>
+    <filterColumn colId="12" showButton="0"/>
+    <filterColumn colId="13" showButton="0"/>
+    <filterColumn colId="14" showButton="0"/>
+    <filterColumn colId="15" showButton="0"/>
+    <filterColumn colId="16" showButton="0"/>
+    <filterColumn colId="18" showButton="0"/>
+    <filterColumn colId="19" showButton="0"/>
+    <filterColumn colId="20" showButton="0"/>
+    <filterColumn colId="21" showButton="0"/>
+    <filterColumn colId="22" showButton="0"/>
+    <filterColumn colId="23" showButton="0"/>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B18">
+    <sortCondition ref="B4:B18"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41" xr:uid="{DF4CABE2-6130-A34D-A3CA-8347E7E96E41}">
+      <formula1>$A$4:$A$18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42" xr:uid="{49543107-F82A-0241-9778-7671BFF1A521}">
+      <formula1>$C$2:$F$2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Añadiendo los géneros al archivo de normalización
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegobeltran/Projects/Movies_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F07BF0-F390-7541-86A1-1DF3B52CF2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5167F0-06CD-A74B-92EE-9A12DB46A244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="500" windowWidth="28160" windowHeight="20760" activeTab="3" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="28160" windowHeight="20760" xr2:uid="{29BFFC22-DD2F-A545-BE55-9FE5A0B360C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="80" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2901" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2908" uniqueCount="1072">
   <si>
     <t>ID</t>
   </si>
@@ -3287,6 +3287,27 @@
   </si>
   <si>
     <t>2019</t>
+  </si>
+  <si>
+    <t>KILLERS OF THE FLOWER MOON</t>
+  </si>
+  <si>
+    <t>LOS ASESINOS DE LA LUNA</t>
+  </si>
+  <si>
+    <t>MARTIN SCORSESE</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>CINE COLOMBIA</t>
+  </si>
+  <si>
+    <t>CINEMA</t>
+  </si>
+  <si>
+    <t>NUESTRO BOGOTÁ</t>
   </si>
 </sst>
 </file>
@@ -3454,7 +3475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3561,830 +3582,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="238">
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -6388,7 +5599,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
@@ -6830,7 +6041,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44</c:v>
@@ -7184,7 +6395,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -7597,7 +6808,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8450,7 +7661,7 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8843,7 +8054,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>14</c:v>
@@ -9203,7 +8414,7 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>33</c:v>
@@ -9978,7 +9189,7 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10129,7 +9340,7 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10576,7 +9787,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>14</c:v>
@@ -10957,7 +10168,7 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>33</c:v>
@@ -26468,7 +25679,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC00E2F0-7487-7C43-AE9A-C0A1988D6274}" name="TablaDinámica2" cacheId="80" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BC00E2F0-7487-7C43-AE9A-C0A1988D6274}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Platform">
   <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -26609,13 +25820,13 @@
     <dataField name="Promedio de Año estreno" fld="8" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="222">
+    <format dxfId="21">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="221">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="220">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -26625,7 +25836,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="219">
+    <format dxfId="18">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -26642,7 +25853,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DDBFC2D8-E807-4D47-84C7-FCF4BECC3BF6}" name="TablaDinámica9" cacheId="80" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="View_place">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DDBFC2D8-E807-4D47-84C7-FCF4BECC3BF6}" name="TablaDinámica9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="View_place">
   <location ref="S3:U7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -26761,13 +25972,13 @@
     <dataField name="Promedio de Minutos" fld="14" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="230">
+    <format dxfId="29">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="229">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="228">
+    <format dxfId="27">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -26776,7 +25987,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="227">
+    <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="12" count="1">
@@ -26785,7 +25996,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="226">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="12" count="1">
@@ -26794,7 +26005,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="225">
+    <format dxfId="24">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="12" count="1">
@@ -26803,7 +26014,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="224">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -26813,7 +26024,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="223">
+    <format dxfId="22">
       <pivotArea field="12" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -26946,7 +26157,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3B88F83-531B-334E-9251-8C8DF41883B3}" name="TablaDinámica1" cacheId="80" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Year_view" colHeaderCaption="Años">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3B88F83-531B-334E-9251-8C8DF41883B3}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Year_view" colHeaderCaption="Años">
   <location ref="K3:Q17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -27066,10 +26277,10 @@
     <dataField name="Count_view" fld="6" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="232">
+    <format dxfId="31">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="231">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -27196,7 +26407,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50BF93F0-D480-9443-8404-6A3A5D7182DB}" name="TablaDinámica4" cacheId="80" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50BF93F0-D480-9443-8404-6A3A5D7182DB}" name="TablaDinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="View_place">
   <location ref="G3:I18" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -27362,13 +26573,13 @@
     <dataField name="Avg_duration(min)" fld="14" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="235">
+    <format dxfId="34">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="234">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="233">
+    <format dxfId="32">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -27409,7 +26620,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74F72E50-9DE8-A64C-850B-D37669125A5B}" name="TablaDinámica3" cacheId="80" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74F72E50-9DE8-A64C-850B-D37669125A5B}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Director">
   <location ref="D3:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -27795,10 +27006,10 @@
     <dataField name="Count_view" fld="6" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="237">
+    <format dxfId="36">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="236">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -27824,43 +27035,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A4A6DBB-95E5-F349-B30E-01F5E818A101}" name="Tabla1" displayName="Tabla1" ref="A2:H14" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A4A6DBB-95E5-F349-B30E-01F5E818A101}" name="Tabla1" displayName="Tabla1" ref="A2:H14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A5A5E420-8F02-0C4A-8221-CB3D62B2C5D9}" name="Year" dataDxfId="216"/>
-    <tableColumn id="2" xr3:uid="{E3ADC4E5-1669-7243-A25F-9784ABBCA501}" name="View count / year" dataDxfId="215"/>
-    <tableColumn id="3" xr3:uid="{C6222808-140C-5743-B272-A6EA41F2B28D}" name="Nº Month" dataDxfId="214"/>
-    <tableColumn id="4" xr3:uid="{AEB3E933-8585-B140-9D83-AD2ED76F835D}" name="Month" dataDxfId="213"/>
-    <tableColumn id="5" xr3:uid="{E881D891-37C9-A54A-A0F7-2F1937B43161}" name="View count / month" dataDxfId="212">
+    <tableColumn id="1" xr3:uid="{A5A5E420-8F02-0C4A-8221-CB3D62B2C5D9}" name="Year" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E3ADC4E5-1669-7243-A25F-9784ABBCA501}" name="View count / year" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{C6222808-140C-5743-B272-A6EA41F2B28D}" name="Nº Month" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{AEB3E933-8585-B140-9D83-AD2ED76F835D}" name="Month" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{E881D891-37C9-A54A-A0F7-2F1937B43161}" name="View count / month" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(Movies!E:E,View_Analysis!C3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9291B7F2-C047-A245-A570-3E65956C06C0}" name="Nº Day of week" dataDxfId="211"/>
-    <tableColumn id="7" xr3:uid="{E63B61D0-FB2A-6543-ABF7-A5A1337847A3}" name="Day of week" dataDxfId="210"/>
-    <tableColumn id="8" xr3:uid="{183AD3B2-31A7-724A-BD7A-6223328AFB58}" name="View count / day of week" dataDxfId="209"/>
+    <tableColumn id="6" xr3:uid="{9291B7F2-C047-A245-A570-3E65956C06C0}" name="Nº Day of week" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{E63B61D0-FB2A-6543-ABF7-A5A1337847A3}" name="Day of week" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{183AD3B2-31A7-724A-BD7A-6223328AFB58}" name="View count / day of week" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B41941F1-754D-FE4C-8D12-1FA64515E1EF}" name="Tabla13" displayName="Tabla13" ref="A37:F52" totalsRowShown="0" headerRowDxfId="208" dataDxfId="207">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B41941F1-754D-FE4C-8D12-1FA64515E1EF}" name="Tabla13" displayName="Tabla13" ref="A37:F52" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:F52">
     <sortCondition descending="1" ref="B38:B52"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{33520D8E-AE00-9D41-8882-149DBBA1153C}" name="Platform" dataDxfId="206"/>
-    <tableColumn id="2" xr3:uid="{6A682448-B962-BE40-A0D0-BA72854AF347}" name="View count / platform" dataDxfId="205">
+    <tableColumn id="1" xr3:uid="{33520D8E-AE00-9D41-8882-149DBBA1153C}" name="Platform" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{6A682448-B962-BE40-A0D0-BA72854AF347}" name="View count / platform" dataDxfId="4">
       <calculatedColumnFormula>COUNTIFS(Movies!$L:$L,Tabla13[[#This Row],[Platform]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{132BBAB9-8C4C-D14F-9A5A-A9ABAA5AE951}" name="2020" dataDxfId="204">
+    <tableColumn id="10" xr3:uid="{132BBAB9-8C4C-D14F-9A5A-A9ABAA5AE951}" name="2020" dataDxfId="3">
       <calculatedColumnFormula>COUNTIFS(Movies!$L:$L,Tabla13[[#This Row],[Platform]],Movies!D:D,Tabla13[[#Headers],[2020]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{5ED70BDD-3B26-ED46-8C04-B73F9AC9A830}" name="2021" dataDxfId="203">
+    <tableColumn id="11" xr3:uid="{5ED70BDD-3B26-ED46-8C04-B73F9AC9A830}" name="2021" dataDxfId="2">
       <calculatedColumnFormula>COUNTIFS(Movies!L:L,Tabla13[[#This Row],[Platform]],Movies!D:D,Tabla13[[#Headers],[2021]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{64A7D1C9-47E2-6448-BBC9-A5F0D98380C0}" name="2022" dataDxfId="202">
+    <tableColumn id="3" xr3:uid="{64A7D1C9-47E2-6448-BBC9-A5F0D98380C0}" name="2022" dataDxfId="1">
       <calculatedColumnFormula>COUNTIFS(Movies!L:L,Tabla13[[#This Row],[Platform]],Movies!D:D,Tabla13[[#Headers],[2022]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E779A56B-D75B-0941-9B7C-5C6B1154326F}" name="2023" dataDxfId="201">
+    <tableColumn id="4" xr3:uid="{E779A56B-D75B-0941-9B7C-5C6B1154326F}" name="2023" dataDxfId="0">
       <calculatedColumnFormula>COUNTIFS(Movies!L:L,Tabla13[[#This Row],[Platform]],Movies!D:D,Tabla13[[#Headers],[2023]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -28166,10 +27377,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE35869-4E62-4D4B-8B4A-6A1A41B2E18E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:O375"/>
+  <dimension ref="A1:O376"/>
   <sheetViews>
-    <sheetView topLeftCell="B337" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D380" sqref="D380"/>
+    <sheetView tabSelected="1" topLeftCell="A345" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I378" sqref="I378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45891,19 +45102,19 @@
         <v>43473</v>
       </c>
       <c r="C348" s="21" t="str">
-        <f t="shared" ref="C348:C375" si="28">CONCATENATE(D348,IF(AND(E348&gt;=1,E348&lt;=9),"0",""),E348)</f>
+        <f t="shared" ref="C348:C376" si="28">CONCATENATE(D348,IF(AND(E348&gt;=1,E348&lt;=9),"0",""),E348)</f>
         <v>201901</v>
       </c>
       <c r="D348" s="7">
-        <f t="shared" ref="D348:D375" si="29">YEAR(B348)</f>
+        <f t="shared" ref="D348:D376" si="29">YEAR(B348)</f>
         <v>2019</v>
       </c>
       <c r="E348" s="7">
-        <f t="shared" ref="E348:E375" si="30">MONTH(B348)</f>
+        <f t="shared" ref="E348:E376" si="30">MONTH(B348)</f>
         <v>1</v>
       </c>
       <c r="F348" s="7">
-        <f t="shared" ref="F348:F375" si="31">WEEKDAY(B348,1)</f>
+        <f t="shared" ref="F348:F376" si="31">WEEKDAY(B348,1)</f>
         <v>3</v>
       </c>
       <c r="G348" s="6" t="s">
@@ -47309,6 +46520,57 @@
       </c>
       <c r="O375" s="7">
         <v>141</v>
+      </c>
+    </row>
+    <row r="376" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A376" s="4">
+        <v>375</v>
+      </c>
+      <c r="B376" s="5">
+        <v>45224</v>
+      </c>
+      <c r="C376" s="21" t="str">
+        <f t="shared" si="28"/>
+        <v>202310</v>
+      </c>
+      <c r="D376" s="7">
+        <f t="shared" si="29"/>
+        <v>2023</v>
+      </c>
+      <c r="E376" s="7">
+        <f t="shared" si="30"/>
+        <v>10</v>
+      </c>
+      <c r="F376" s="7">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="G376" s="6" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H376" s="6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I376" s="7">
+        <v>2023</v>
+      </c>
+      <c r="J376" s="8" t="s">
+        <v>1067</v>
+      </c>
+      <c r="K376" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="L376" s="8" t="s">
+        <v>1069</v>
+      </c>
+      <c r="M376" s="8" t="s">
+        <v>1070</v>
+      </c>
+      <c r="N376" s="8" t="s">
+        <v>1071</v>
+      </c>
+      <c r="O376" s="7">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -47420,22 +46682,22 @@
       <c r="A4" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="38">
         <v>1941</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4">
         <v>10</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4">
         <v>293</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="38">
         <v>122.00682593856655</v>
       </c>
       <c r="K4" s="11" t="s">
@@ -47462,10 +46724,10 @@
       <c r="S4" s="12" t="s">
         <v>937</v>
       </c>
-      <c r="T4" s="44">
+      <c r="T4" s="40">
         <v>0.20053475935828877</v>
       </c>
-      <c r="U4" s="42">
+      <c r="U4" s="38">
         <v>127.96</v>
       </c>
     </row>
@@ -47473,52 +46735,52 @@
       <c r="A5" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="38">
         <v>1972</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5">
         <v>6</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5">
         <v>17</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="38">
         <v>123.23529411764706</v>
       </c>
       <c r="K5" s="37" t="s">
         <v>979</v>
       </c>
-      <c r="L5" s="40">
+      <c r="L5">
         <v>11</v>
       </c>
-      <c r="M5" s="40">
+      <c r="M5">
         <v>16</v>
       </c>
-      <c r="N5" s="40">
+      <c r="N5">
         <v>10</v>
       </c>
-      <c r="O5" s="40">
+      <c r="O5">
         <v>8</v>
       </c>
-      <c r="P5" s="40">
+      <c r="P5">
         <v>4</v>
       </c>
-      <c r="Q5" s="40">
+      <c r="Q5">
         <v>49</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>938</v>
       </c>
-      <c r="T5" s="44">
+      <c r="T5" s="40">
         <v>4.8128342245989303E-2</v>
       </c>
-      <c r="U5" s="42">
+      <c r="U5" s="38">
         <v>136.44444444444446</v>
       </c>
     </row>
@@ -47526,52 +46788,52 @@
       <c r="A6" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="38">
         <v>1978.6666666666667</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6">
         <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6">
         <v>12</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="38">
         <v>113.66666666666667</v>
       </c>
       <c r="K6" s="37" t="s">
         <v>980</v>
       </c>
-      <c r="L6" s="40">
+      <c r="L6">
         <v>7</v>
       </c>
-      <c r="M6" s="40">
+      <c r="M6">
         <v>11</v>
       </c>
-      <c r="N6" s="40">
+      <c r="N6">
         <v>8</v>
       </c>
-      <c r="O6" s="40">
+      <c r="O6">
         <v>5</v>
       </c>
-      <c r="P6" s="40">
+      <c r="P6">
         <v>5</v>
       </c>
-      <c r="Q6" s="40">
+      <c r="Q6">
         <v>36</v>
       </c>
       <c r="S6" s="12" t="s">
         <v>939</v>
       </c>
-      <c r="T6" s="44">
+      <c r="T6" s="40">
         <v>0.75133689839572193</v>
       </c>
-      <c r="U6" s="42">
+      <c r="U6" s="38">
         <v>121.36654804270462</v>
       </c>
     </row>
@@ -47579,52 +46841,52 @@
       <c r="A7" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="38">
         <v>1991.4772727272727</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7">
         <v>6</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7">
         <v>10</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="38">
         <v>127.9</v>
       </c>
       <c r="K7" s="37" t="s">
         <v>981</v>
       </c>
-      <c r="L7" s="40">
+      <c r="L7">
         <v>7</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7">
         <v>16</v>
       </c>
-      <c r="N7" s="40">
+      <c r="N7">
         <v>7</v>
       </c>
-      <c r="O7" s="40">
+      <c r="O7">
         <v>2</v>
       </c>
-      <c r="P7" s="40">
+      <c r="P7">
         <v>2</v>
       </c>
-      <c r="Q7" s="40">
+      <c r="Q7">
         <v>34</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="S7" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="T7" s="43">
+      <c r="T7" s="39">
         <v>1</v>
       </c>
-      <c r="U7" s="42">
+      <c r="U7" s="38">
         <v>123.4144385026738</v>
       </c>
     </row>
@@ -47632,43 +46894,43 @@
       <c r="A8" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8" s="38">
         <v>1995.4285714285713</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8">
         <v>5</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="H8" s="40">
+      <c r="H8">
         <v>7</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="38">
         <v>130</v>
       </c>
       <c r="K8" s="37" t="s">
         <v>982</v>
       </c>
-      <c r="L8" s="40">
+      <c r="L8">
         <v>22</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8">
         <v>13</v>
       </c>
-      <c r="N8" s="40">
+      <c r="N8">
         <v>13</v>
       </c>
-      <c r="O8" s="40">
+      <c r="O8">
         <v>6</v>
       </c>
-      <c r="P8" s="40">
+      <c r="P8">
         <v>3</v>
       </c>
-      <c r="Q8" s="40">
+      <c r="Q8">
         <v>57</v>
       </c>
     </row>
@@ -47676,43 +46938,43 @@
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="38">
         <v>2000.9402985074628</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9">
         <v>5</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>995</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="38">
         <v>111.83333333333333</v>
       </c>
       <c r="K9" s="37" t="s">
         <v>983</v>
       </c>
-      <c r="L9" s="40">
+      <c r="L9">
         <v>16</v>
       </c>
-      <c r="M9" s="40">
+      <c r="M9">
         <v>13</v>
       </c>
-      <c r="N9" s="40">
+      <c r="N9">
         <v>7</v>
       </c>
-      <c r="O9" s="40">
+      <c r="O9">
         <v>2</v>
       </c>
-      <c r="P9" s="40">
+      <c r="P9">
         <v>1</v>
       </c>
-      <c r="Q9" s="40">
+      <c r="Q9">
         <v>39</v>
       </c>
     </row>
@@ -47720,43 +46982,43 @@
       <c r="A10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="38">
         <v>2003.2112676056338</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10">
         <v>5</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>578</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10">
         <v>5</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="38">
         <v>137.6</v>
       </c>
       <c r="K10" s="37" t="s">
         <v>984</v>
       </c>
-      <c r="L10" s="40">
+      <c r="L10">
         <v>3</v>
       </c>
-      <c r="M10" s="40">
+      <c r="M10">
         <v>12</v>
       </c>
-      <c r="N10" s="40">
+      <c r="N10">
         <v>7</v>
       </c>
-      <c r="O10" s="40">
+      <c r="O10">
         <v>5</v>
       </c>
-      <c r="P10" s="40">
+      <c r="P10">
         <v>3</v>
       </c>
-      <c r="Q10" s="40">
+      <c r="Q10">
         <v>30</v>
       </c>
     </row>
@@ -47764,43 +47026,43 @@
       <c r="A11" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="38">
         <v>2004.9166666666667</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>654</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11">
         <v>5</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>685</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11">
         <v>5</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="38">
         <v>150.6</v>
       </c>
       <c r="K11" s="37" t="s">
         <v>985</v>
       </c>
-      <c r="L11" s="40">
+      <c r="L11">
         <v>5</v>
       </c>
-      <c r="M11" s="40">
+      <c r="M11">
         <v>11</v>
       </c>
-      <c r="N11" s="40">
+      <c r="N11">
         <v>8</v>
       </c>
-      <c r="O11" s="40">
+      <c r="O11">
         <v>2</v>
       </c>
-      <c r="P11" s="40">
+      <c r="P11">
         <v>5</v>
       </c>
-      <c r="Q11" s="40">
+      <c r="Q11">
         <v>31</v>
       </c>
     </row>
@@ -47808,43 +47070,43 @@
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="42">
+      <c r="B12" s="38">
         <v>2008.3611111111111</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12">
         <v>4</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>827</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12">
         <v>4</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="38">
         <v>134.25</v>
       </c>
       <c r="K12" s="37" t="s">
         <v>986</v>
       </c>
-      <c r="L12" s="40">
+      <c r="L12">
         <v>2</v>
       </c>
-      <c r="M12" s="40">
+      <c r="M12">
         <v>10</v>
       </c>
-      <c r="N12" s="40">
+      <c r="N12">
         <v>8</v>
       </c>
-      <c r="O12" s="40">
+      <c r="O12">
         <v>2</v>
       </c>
-      <c r="P12" s="40">
+      <c r="P12">
         <v>1</v>
       </c>
-      <c r="Q12" s="40">
+      <c r="Q12">
         <v>23</v>
       </c>
     </row>
@@ -47852,41 +47114,40 @@
       <c r="A13" s="12" t="s">
         <v>577</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="38">
         <v>2018</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13">
         <v>4</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>625</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="38">
         <v>142.33333333333334</v>
       </c>
       <c r="K13" s="37" t="s">
         <v>987</v>
       </c>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40">
+      <c r="M13">
         <v>7</v>
       </c>
-      <c r="N13" s="40">
+      <c r="N13">
         <v>7</v>
       </c>
-      <c r="O13" s="40">
+      <c r="O13">
         <v>3</v>
       </c>
-      <c r="P13" s="40">
+      <c r="P13">
         <v>1</v>
       </c>
-      <c r="Q13" s="40">
+      <c r="Q13">
         <v>18</v>
       </c>
     </row>
@@ -47894,43 +47155,43 @@
       <c r="A14" s="12" t="s">
         <v>996</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14" s="38">
         <v>2018</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14">
         <v>56</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>877</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="38">
         <v>180.5</v>
       </c>
       <c r="K14" s="37" t="s">
         <v>988</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14">
         <v>2</v>
       </c>
-      <c r="M14" s="40">
+      <c r="M14">
         <v>10</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14">
         <v>6</v>
       </c>
-      <c r="O14" s="40">
+      <c r="O14">
         <v>2</v>
       </c>
-      <c r="P14" s="40">
+      <c r="P14">
         <v>2</v>
       </c>
-      <c r="Q14" s="40">
+      <c r="Q14">
         <v>22</v>
       </c>
     </row>
@@ -47938,33 +47199,31 @@
       <c r="A15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15" s="38">
         <v>2019.8833333333334</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>994</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="38">
         <v>110.5</v>
       </c>
       <c r="K15" s="37" t="s">
         <v>989</v>
       </c>
-      <c r="L15" s="40">
+      <c r="L15">
         <v>3</v>
       </c>
-      <c r="M15" s="40">
+      <c r="M15">
         <v>7</v>
       </c>
-      <c r="N15" s="40">
+      <c r="N15">
         <v>4</v>
       </c>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40">
+      <c r="Q15">
         <v>14</v>
       </c>
     </row>
@@ -47972,35 +47231,34 @@
       <c r="A16" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16" s="38">
         <v>2021.3333333333333</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16">
         <v>2</v>
       </c>
-      <c r="I16" s="42">
+      <c r="I16" s="38">
         <v>125</v>
       </c>
       <c r="K16" s="37" t="s">
         <v>990</v>
       </c>
-      <c r="L16" s="40">
+      <c r="L16">
         <v>6</v>
       </c>
-      <c r="M16" s="40">
+      <c r="M16">
         <v>9</v>
       </c>
-      <c r="N16" s="40">
+      <c r="N16">
         <v>5</v>
       </c>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40">
+      <c r="P16">
         <v>1</v>
       </c>
-      <c r="Q16" s="40">
+      <c r="Q16">
         <v>21</v>
       </c>
     </row>
@@ -48008,37 +47266,37 @@
       <c r="A17" s="12" t="s">
         <v>604</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="38">
         <v>2021.6666666666667</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>516</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="38">
         <v>149</v>
       </c>
-      <c r="K17" s="45" t="s">
+      <c r="K17" s="37" t="s">
         <v>890</v>
       </c>
-      <c r="L17" s="40">
+      <c r="L17">
         <v>84</v>
       </c>
-      <c r="M17" s="40">
+      <c r="M17">
         <v>135</v>
       </c>
-      <c r="N17" s="40">
+      <c r="N17">
         <v>90</v>
       </c>
-      <c r="O17" s="40">
+      <c r="O17">
         <v>37</v>
       </c>
-      <c r="P17" s="40">
+      <c r="P17">
         <v>28</v>
       </c>
-      <c r="Q17" s="40">
+      <c r="Q17">
         <v>374</v>
       </c>
     </row>
@@ -48046,16 +47304,16 @@
       <c r="A18" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18" s="38">
         <v>2022</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18">
         <v>370</v>
       </c>
-      <c r="I18" s="42">
+      <c r="I18" s="38">
         <v>123.24864864864865</v>
       </c>
     </row>
@@ -48063,15 +47321,15 @@
       <c r="A19" s="12" t="s">
         <v>660</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19" s="38">
         <v>2022</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="38">
         <v>2004.566844919786</v>
       </c>
     </row>
@@ -48104,16 +47362,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>932</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:11" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
@@ -48235,7 +47493,7 @@
       </c>
       <c r="B6" s="14">
         <f>COUNTIF(Movies!D:D,View_Analysis!A6)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="14">
         <v>4</v>
@@ -48255,7 +47513,7 @@
       </c>
       <c r="H6" s="14">
         <f>COUNTIF(Movies!F:F,View_Analysis!F6)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -48375,7 +47633,7 @@
       </c>
       <c r="E12" s="14">
         <f>COUNTIF(Movies!E:E,View_Analysis!C12)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -48416,14 +47674,14 @@
       <c r="H14" s="14"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="41" t="s">
         <v>934</v>
       </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
     </row>
@@ -48553,7 +47811,7 @@
       </c>
       <c r="B42" s="14">
         <f>COUNTIFS(Movies!$L:$L,Tabla13[[#This Row],[Platform]])</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42" s="14">
         <f>COUNTIFS(Movies!$L:$L,Tabla13[[#This Row],[Platform]],Movies!D:D,Tabla13[[#Headers],[2020]])</f>
@@ -48569,7 +47827,7 @@
       </c>
       <c r="F42" s="14">
         <f>COUNTIFS(Movies!L:L,Tabla13[[#This Row],[Platform]],Movies!D:D,Tabla13[[#Headers],[2023]])</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -48885,7 +48143,7 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="96" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="96" workbookViewId="0">
       <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
@@ -49138,7 +48396,7 @@
       </c>
       <c r="H62" s="31">
         <f>COUNTIF(Movies!F:F,$F62)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I62" s="32">
         <v>201904</v>
@@ -49157,7 +48415,7 @@
       </c>
       <c r="B63" s="31">
         <f>COUNTIF(Movies!D:D,$A63)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C63" s="31">
         <v>5</v>
@@ -49323,7 +48581,7 @@
       </c>
       <c r="E68" s="31">
         <f>COUNTIF(Movies!E:E,$C68)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F68" s="31"/>
       <c r="G68" s="31"/>
@@ -50230,7 +49488,7 @@
       </c>
       <c r="K116" s="31">
         <f>COUNTIF(Movies!C:C,$I116)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="9:11" x14ac:dyDescent="0.2">
@@ -50291,35 +49549,35 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B1" s="22"/>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="42" t="s">
         <v>969</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42" t="s">
         <v>970</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="38" t="s">
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="41" t="s">
         <v>971</v>
       </c>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="C2" s="36">
@@ -51677,7 +50935,7 @@
       </c>
       <c r="B14">
         <f>COUNTIF(Movies!$L:$L,$A14)</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="22">
         <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$D:$D,Hoja1!C$3)</f>
@@ -51693,7 +50951,7 @@
       </c>
       <c r="F14" s="22">
         <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$D:$D,Hoja1!F$3)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G14" s="22">
         <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!G$3)</f>
@@ -51733,7 +50991,7 @@
       </c>
       <c r="P14" s="22">
         <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!P$3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q14" s="22">
         <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$E:$E,Hoja1!Q$3)</f>
@@ -51757,7 +51015,7 @@
       </c>
       <c r="V14" s="22">
         <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!V$3)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W14" s="22">
         <f>COUNTIFS(Movies!$L:$L,Hoja1!$A14,Movies!$F:$F,Hoja1!W$3)</f>
@@ -52398,7 +51656,7 @@
       </c>
       <c r="C22">
         <f>VLOOKUP(B22,$A$4:$B$18,2,0)</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="22">
         <f>INDEX($C$4:$F$18,MATCH($B$22,$A$4:$A$18,0),MATCH(D$20,$C$3:$F$3,0))</f>
@@ -52414,7 +51672,7 @@
       </c>
       <c r="G22" s="22">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H22" s="22">
         <f>INDEX($G$4:$R$18,MATCH($B$22,$A$4:$A$18,0),MATCH(H$20,$G$3:$R$3,0))</f>
@@ -52454,7 +51712,7 @@
       </c>
       <c r="Q22" s="22">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R22" s="22">
         <f t="shared" si="1"/>
@@ -52478,7 +51736,7 @@
       </c>
       <c r="W22">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X22">
         <f t="shared" si="2"/>

</xml_diff>